<commit_message>
added Bret's edits, started thinking of Model results Sup
</commit_message>
<xml_diff>
--- a/doc/MainTables.xlsx
+++ b/doc/MainTables.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Table1 Strain.Info" sheetId="3" r:id="rId1"/>
     <sheet name="Table 2 Models" sheetId="4" r:id="rId2"/>
     <sheet name="Table 3 MLH1" sheetId="1" r:id="rId3"/>
     <sheet name="Table 4 DMC1" sheetId="2" r:id="rId4"/>
+    <sheet name="Supplemental Table (Model)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="115">
   <si>
     <t>Species</t>
   </si>
@@ -215,12 +216,6 @@
     <t>subspecies * strain</t>
   </si>
   <si>
-    <t>strains with observations of both sexes</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -312,12 +307,6 @@
   </si>
   <si>
     <t>Geographic                              Origin</t>
-  </si>
-  <si>
-    <t>sex specific mouse averages             (male or female)</t>
-  </si>
-  <si>
-    <t>sex specific mouse averages                    (male or female)</t>
   </si>
   <si>
     <t>Subspecies</t>
@@ -465,6 +454,30 @@
   </si>
   <si>
     <t>TOM/TUA</t>
+  </si>
+  <si>
+    <t>Dataset(s)</t>
+  </si>
+  <si>
+    <t>Dependent Variable(s)</t>
+  </si>
+  <si>
+    <t>mouse average</t>
+  </si>
+  <si>
+    <t>female mouse average</t>
+  </si>
+  <si>
+    <t>male mouse average</t>
+  </si>
+  <si>
+    <t>females and males from 8 strains</t>
+  </si>
+  <si>
+    <t>females from 8 strains</t>
+  </si>
+  <si>
+    <t>males from 12 strains</t>
   </si>
 </sst>
 </file>
@@ -880,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1171,37 +1184,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1247,12 +1248,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1290,6 +1285,63 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1574,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1592,13 +1644,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>51</v>
@@ -1613,7 +1665,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="91" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E2" s="103" t="s">
         <v>44</v>
@@ -1622,22 +1674,22 @@
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="119"/>
       <c r="B3" s="106" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="114" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="119"/>
       <c r="B4" s="106" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="114" t="s">
         <v>41</v>
@@ -1646,22 +1698,22 @@
         <v>42</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="120"/>
       <c r="B5" s="99" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="115" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="94" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" s="105" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1669,91 +1721,91 @@
         <v>14</v>
       </c>
       <c r="B6" s="95" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="113" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E6" s="103" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
       <c r="B7" s="98" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" s="114" t="s">
         <v>56</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="122"/>
       <c r="B8" s="96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="114" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="92" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8" s="104" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="122"/>
       <c r="B9" s="96" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="114" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="89" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E9" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="122"/>
       <c r="B10" s="98" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="114" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E10" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="123"/>
       <c r="B11" s="97" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C11" s="115" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E11" s="105" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1761,31 +1813,31 @@
         <v>18</v>
       </c>
       <c r="B12" s="99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="113" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="93" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="125"/>
       <c r="B13" s="99" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="115" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="93" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E13" s="104" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1793,7 +1845,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="101" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="113" t="s">
         <v>38</v>
@@ -1802,22 +1854,22 @@
         <v>40</v>
       </c>
       <c r="E14" s="103" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="125"/>
       <c r="B15" s="100" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" s="115" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="100" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E15" s="105" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1825,16 +1877,16 @@
         <v>21</v>
       </c>
       <c r="B16" s="102" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="113" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="112" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" s="105" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1842,16 +1894,16 @@
         <v>23</v>
       </c>
       <c r="B17" s="91" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" s="116" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" s="112" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="103" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1859,7 +1911,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="110" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" s="117" t="s">
         <v>52</v>
@@ -1868,7 +1920,7 @@
         <v>40</v>
       </c>
       <c r="E18" s="111" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1908,199 +1960,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="160" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="80" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="80" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="167" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="161" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="E2" s="84" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="130"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="38" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="127"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="60"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="131"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="38" t="s">
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="128"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="60"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="129" t="s">
+      <c r="E4" s="60"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="132" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="81" t="s">
+      <c r="B5" s="170" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="161" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="84"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
-      <c r="B6" s="133"/>
-      <c r="C6" s="82" t="s">
+      <c r="E5" s="84"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="127"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="60"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="82" t="s">
+      <c r="E6" s="60"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="127"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="60"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="130"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="82" t="s">
+      <c r="E7" s="60"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="127"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="60"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
-      <c r="C9" s="82" t="s">
+      <c r="E8" s="60"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="127"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="60"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="83" t="s">
+      <c r="E9" s="60"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="128"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="85"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="129" t="s">
+      <c r="E10" s="85"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="132" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="170" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="161" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="84"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="82" t="s">
+      <c r="E11" s="84"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="127"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="83" t="s">
+      <c r="E12" s="60"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="128"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="85"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="129" t="s">
+      <c r="E13" s="85"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="132" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="173" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="164" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="84"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
-      <c r="B15" s="133"/>
-      <c r="C15" s="82" t="s">
+      <c r="E14" s="84"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="127"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="60"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="131"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="83" t="s">
+      <c r="E15" s="60"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="128"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="85"/>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="129" t="s">
+      <c r="E16" s="85"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="126" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="176" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="164" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="86"/>
-    </row>
-    <row r="18" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="131"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="87"/>
+      <c r="E17" s="86"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="128"/>
+      <c r="B18" s="174"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="87"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="175"/>
+      <c r="C19" s="166"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="177" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="164" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="178"/>
+      <c r="C21" s="166"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="177" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="164" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="178"/>
+      <c r="C23" s="166"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B17:B18"/>
+  <mergeCells count="8">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A17:A18"/>
@@ -2132,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>1</v>
@@ -2160,13 +2269,13 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="152" t="s">
+      <c r="C2" s="129" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -2192,9 +2301,9 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="143"/>
-      <c r="B3" s="147"/>
-      <c r="C3" s="153"/>
+      <c r="A3" s="139"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="130"/>
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
@@ -2218,9 +2327,9 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="143"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="152" t="s">
+      <c r="A4" s="139"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="129" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -2246,9 +2355,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="143"/>
-      <c r="B5" s="147"/>
-      <c r="C5" s="153"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="130"/>
       <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
@@ -2272,9 +2381,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="143"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="152" t="s">
+      <c r="A6" s="139"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="129" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -2300,9 +2409,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="147"/>
-      <c r="C7" s="154"/>
+      <c r="A7" s="139"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="148"/>
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
@@ -2336,8 +2445,8 @@
       <c r="U7" s="36"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="143"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="144"/>
       <c r="C8" s="34" t="s">
         <v>41</v>
       </c>
@@ -2374,11 +2483,11 @@
       <c r="U8" s="42"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="146" t="s">
+      <c r="A9" s="139"/>
+      <c r="B9" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C9" s="131" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -2404,9 +2513,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
-      <c r="B10" s="147"/>
-      <c r="C10" s="136"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
@@ -2430,9 +2539,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="143"/>
-      <c r="B11" s="147"/>
-      <c r="C11" s="152" t="s">
+      <c r="A11" s="139"/>
+      <c r="B11" s="143"/>
+      <c r="C11" s="129" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -2458,9 +2567,9 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
-      <c r="B12" s="147"/>
-      <c r="C12" s="153"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="130"/>
       <c r="D12" s="15" t="s">
         <v>11</v>
       </c>
@@ -2484,9 +2593,9 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
-      <c r="B13" s="147"/>
-      <c r="C13" s="152" t="s">
+      <c r="A13" s="139"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="129" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -2512,9 +2621,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="147"/>
-      <c r="C14" s="153"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="130"/>
       <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
@@ -2538,8 +2647,8 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="147"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="49" t="s">
         <v>56</v>
       </c>
@@ -2566,8 +2675,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="147"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="49" t="s">
         <v>37</v>
       </c>
@@ -2594,8 +2703,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="148"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="144"/>
       <c r="C17" s="48" t="s">
         <v>43</v>
       </c>
@@ -2622,11 +2731,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="143"/>
-      <c r="B18" s="146" t="s">
+      <c r="A18" s="139"/>
+      <c r="B18" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="144" t="s">
+      <c r="C18" s="140" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="66" t="s">
@@ -2652,9 +2761,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="143"/>
-      <c r="B19" s="147"/>
-      <c r="C19" s="145"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="141"/>
       <c r="D19" s="67" t="s">
         <v>11</v>
       </c>
@@ -2678,8 +2787,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="148"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="144"/>
       <c r="C20" s="48" t="s">
         <v>39</v>
       </c>
@@ -2706,11 +2815,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
-      <c r="B21" s="149" t="s">
+      <c r="A21" s="139"/>
+      <c r="B21" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="150" t="s">
+      <c r="C21" s="146" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="50" t="s">
@@ -2736,9 +2845,9 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="149"/>
-      <c r="C22" s="151"/>
+      <c r="A22" s="139"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="32" t="s">
         <v>11</v>
       </c>
@@ -2762,9 +2871,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
-      <c r="B23" s="149"/>
-      <c r="C23" s="135" t="s">
+      <c r="A23" s="139"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="131" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="31" t="s">
@@ -2790,9 +2899,9 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="140"/>
-      <c r="B24" s="149"/>
-      <c r="C24" s="136"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="132"/>
       <c r="D24" s="33" t="s">
         <v>11</v>
       </c>
@@ -2816,11 +2925,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="137" t="s">
+      <c r="A25" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="138"/>
-      <c r="C25" s="135" t="s">
+      <c r="B25" s="134"/>
+      <c r="C25" s="131" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="32" t="s">
@@ -2846,9 +2955,9 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="139"/>
-      <c r="B26" s="140"/>
-      <c r="C26" s="136"/>
+      <c r="A26" s="135"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="132"/>
       <c r="D26" s="32" t="s">
         <v>11</v>
       </c>
@@ -2872,11 +2981,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="137" t="s">
+      <c r="A27" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="138"/>
-      <c r="C27" s="135" t="s">
+      <c r="B27" s="134"/>
+      <c r="C27" s="131" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="31" t="s">
@@ -2902,9 +3011,9 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="139"/>
-      <c r="B28" s="140"/>
-      <c r="C28" s="136"/>
+      <c r="A28" s="135"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="33" t="s">
         <v>11</v>
       </c>
@@ -2928,10 +3037,10 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="141" t="s">
+      <c r="A29" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="142"/>
+      <c r="B29" s="138"/>
       <c r="C29" s="48" t="s">
         <v>52</v>
       </c>
@@ -2959,12 +3068,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="A27:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A2:A24"/>
     <mergeCell ref="C18:C19"/>
@@ -2978,6 +3081,12 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="A27:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3004,26 +3113,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="129" t="s">
+      <c r="B1" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="C1" s="149" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="158" t="s">
+      <c r="D1" s="150"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="159"/>
-      <c r="H1" s="160"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="154"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="165"/>
-      <c r="B2" s="131"/>
+      <c r="A2" s="159"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="5" t="s">
         <v>27</v>
       </c>
@@ -3044,11 +3153,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="155" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" s="7">
         <v>21</v>
@@ -3070,9 +3179,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="161"/>
+      <c r="A4" s="155"/>
       <c r="B4" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="7">
         <v>19</v>
@@ -3094,9 +3203,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="161"/>
+      <c r="A5" s="155"/>
       <c r="B5" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -3118,11 +3227,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="156" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" s="11">
         <v>18</v>
@@ -3144,9 +3253,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="163"/>
+      <c r="A7" s="157"/>
       <c r="B7" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" s="15">
         <v>17</v>
@@ -3179,4 +3288,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removing old files, Model results
</commit_message>
<xml_diff>
--- a/doc/MainTables.xlsx
+++ b/doc/MainTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Table1 Strain.Info" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,19 @@
     <sheet name="Table 3 MLH1" sheetId="1" r:id="rId3"/>
     <sheet name="Table 4 DMC1" sheetId="2" r:id="rId4"/>
     <sheet name="Supplemental Table (Model)" sheetId="5" r:id="rId5"/>
+    <sheet name="MLH1_M2" sheetId="6" r:id="rId6"/>
+    <sheet name="MLH1_M3" sheetId="7" r:id="rId7"/>
+    <sheet name="MLH1_M4.M5_female" sheetId="8" r:id="rId8"/>
+    <sheet name="MLH1_M4.M5_male" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="MLH1_M2_glm" localSheetId="5">MLH1_M2!$A$1:$E$17</definedName>
+    <definedName name="MLH1_M3_glm" localSheetId="6">MLH1_M3!$A$1:$E$17</definedName>
+    <definedName name="MLH1_M4_female_glm" localSheetId="7">MLH1_M4.M5_female!$A$1:$E$9</definedName>
+    <definedName name="MLH1_M4_male_glm" localSheetId="8">MLH1_M4.M5_male!$A$1:$E$13</definedName>
+    <definedName name="MLH1_M5_female_glm" localSheetId="7">MLH1_M4.M5_female!$A$11:$E$19</definedName>
+    <definedName name="MLH1_M5_male_glm" localSheetId="8">MLH1_M4.M5_male!$A$15:$E$27</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,8 +39,79 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="MLH1_M2_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M2_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="MLH1_M3_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M3_glm.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="MLH1_M4_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_female_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="MLH1_M4_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_male_glm.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="MLH1_M5_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_female_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="MLH1_M5_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_male_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="143">
   <si>
     <t>Species</t>
   </si>
@@ -478,6 +561,90 @@
   </si>
   <si>
     <t>males from 12 strains</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Std. Error</t>
+  </si>
+  <si>
+    <t>t value</t>
+  </si>
+  <si>
+    <t>Pr(&gt;|t|)</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>subspMusc</t>
+  </si>
+  <si>
+    <t>subspMol</t>
+  </si>
+  <si>
+    <t>sexmale</t>
+  </si>
+  <si>
+    <t>strainG</t>
+  </si>
+  <si>
+    <t>strainLEW</t>
+  </si>
+  <si>
+    <t>strainPWD</t>
+  </si>
+  <si>
+    <t>strainMSM</t>
+  </si>
+  <si>
+    <t>strainSKIVE</t>
+  </si>
+  <si>
+    <t>subspMusc:sexmale</t>
+  </si>
+  <si>
+    <t>subspMol:sexmale</t>
+  </si>
+  <si>
+    <t>sexmale:strainG</t>
+  </si>
+  <si>
+    <t>sexmale:strainLEW</t>
+  </si>
+  <si>
+    <t>sexmale:strainPWD</t>
+  </si>
+  <si>
+    <t>sexmale:strainMSM</t>
+  </si>
+  <si>
+    <t>sexmale:strainSKIVE</t>
+  </si>
+  <si>
+    <t>strainMOLF</t>
+  </si>
+  <si>
+    <t>strainKAZ</t>
+  </si>
+  <si>
+    <t>sexmale:strainMOLF</t>
+  </si>
+  <si>
+    <t>sexmale:strainKAZ</t>
+  </si>
+  <si>
+    <t>strainPERC</t>
+  </si>
+  <si>
+    <t>strainTOM</t>
+  </si>
+  <si>
+    <t>strainAST</t>
+  </si>
+  <si>
+    <t>strainCZECH</t>
   </si>
 </sst>
 </file>
@@ -893,7 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1160,6 +1327,45 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,6 +1390,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,64 +1408,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1286,63 +1510,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1359,6 +1527,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M2_glm" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M3_glm" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1657,7 +1849,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="131" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="90"/>
@@ -1672,7 +1864,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
+      <c r="A3" s="132"/>
       <c r="B3" s="106" t="s">
         <v>80</v>
       </c>
@@ -1687,7 +1879,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
+      <c r="A4" s="132"/>
       <c r="B4" s="106" t="s">
         <v>78</v>
       </c>
@@ -1702,7 +1894,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="120"/>
+      <c r="A5" s="133"/>
       <c r="B5" s="99" t="s">
         <v>86</v>
       </c>
@@ -1717,7 +1909,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="134" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="95" t="s">
@@ -1734,7 +1926,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="98" t="s">
         <v>83</v>
       </c>
@@ -1749,7 +1941,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="96" t="s">
         <v>69</v>
       </c>
@@ -1764,7 +1956,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
+      <c r="A9" s="135"/>
       <c r="B9" s="96" t="s">
         <v>65</v>
       </c>
@@ -1779,7 +1971,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="98" t="s">
         <v>79</v>
       </c>
@@ -1794,7 +1986,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="123"/>
+      <c r="A11" s="136"/>
       <c r="B11" s="97" t="s">
         <v>106</v>
       </c>
@@ -1809,7 +2001,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="137" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="99" t="s">
@@ -1826,7 +2018,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
+      <c r="A13" s="138"/>
       <c r="B13" s="99" t="s">
         <v>81</v>
       </c>
@@ -1841,7 +2033,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="137" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="101" t="s">
@@ -1858,7 +2050,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="100" t="s">
         <v>87</v>
       </c>
@@ -1979,10 +2171,10 @@
       <c r="A1" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="160" t="s">
+      <c r="C1" s="118" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="80" t="s">
@@ -1993,13 +2185,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="139" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="161" t="s">
+      <c r="C2" s="119" t="s">
         <v>109</v>
       </c>
       <c r="D2" s="37" t="s">
@@ -2010,31 +2202,31 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="127"/>
-      <c r="B3" s="168"/>
-      <c r="C3" s="162"/>
+      <c r="A3" s="143"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="120"/>
       <c r="D3" s="38" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="60"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
-      <c r="B4" s="169"/>
-      <c r="C4" s="163"/>
+      <c r="A4" s="144"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="38" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="145" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="161" t="s">
+      <c r="C5" s="119" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -2043,58 +2235,58 @@
       <c r="E5" s="84"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="127"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="162"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="120"/>
       <c r="D6" s="82" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="162"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="120"/>
       <c r="D7" s="82" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="60"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="162"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="120"/>
       <c r="D8" s="82" t="s">
         <v>58</v>
       </c>
       <c r="E8" s="60"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="127"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="162"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="120"/>
       <c r="D9" s="82" t="s">
         <v>59</v>
       </c>
       <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="128"/>
-      <c r="B10" s="172"/>
-      <c r="C10" s="163"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="121"/>
       <c r="D10" s="83" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="85"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="126" t="s">
+      <c r="A11" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="170" t="s">
+      <c r="B11" s="145" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="161" t="s">
+      <c r="C11" s="119" t="s">
         <v>109</v>
       </c>
       <c r="D11" s="81" t="s">
@@ -2103,31 +2295,31 @@
       <c r="E11" s="84"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="127"/>
-      <c r="B12" s="171"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="120"/>
       <c r="D12" s="82" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="60"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="128"/>
-      <c r="B13" s="172"/>
-      <c r="C13" s="163"/>
+      <c r="A13" s="144"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="121"/>
       <c r="D13" s="83" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="85"/>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="173" t="s">
+      <c r="B14" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="164" t="s">
+      <c r="C14" s="122" t="s">
         <v>110</v>
       </c>
       <c r="D14" s="81" t="s">
@@ -2136,31 +2328,31 @@
       <c r="E14" s="84"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="127"/>
-      <c r="B15" s="174"/>
-      <c r="C15" s="165"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="123"/>
       <c r="D15" s="82" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="60"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="128"/>
-      <c r="B16" s="175"/>
-      <c r="C16" s="166"/>
+      <c r="A16" s="144"/>
+      <c r="B16" s="127"/>
+      <c r="C16" s="124"/>
       <c r="D16" s="83" t="s">
         <v>61</v>
       </c>
       <c r="E16" s="85"/>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="126" t="s">
+      <c r="A17" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="176" t="s">
+      <c r="B17" s="128" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="164" t="s">
+      <c r="C17" s="122" t="s">
         <v>111</v>
       </c>
       <c r="D17" s="31" t="s">
@@ -2169,42 +2361,43 @@
       <c r="E17" s="86"/>
     </row>
     <row r="18" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="128"/>
-      <c r="B18" s="174"/>
-      <c r="C18" s="165"/>
+      <c r="A18" s="144"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="33"/>
       <c r="E18" s="87"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="175"/>
-      <c r="C19" s="166"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="124"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="177" t="s">
+      <c r="B20" s="129" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="164" t="s">
+      <c r="C20" s="122" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="178"/>
-      <c r="C21" s="166"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="124"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="177" t="s">
+      <c r="B22" s="129" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="164" t="s">
+      <c r="C22" s="122" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="178"/>
-      <c r="C23" s="166"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A10"/>
@@ -2212,7 +2405,6 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2269,13 +2461,13 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="129" t="s">
+      <c r="C2" s="163" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -2301,9 +2493,9 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="130"/>
+      <c r="A3" s="151"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="164"/>
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
@@ -2327,9 +2519,9 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="139"/>
-      <c r="B4" s="143"/>
-      <c r="C4" s="129" t="s">
+      <c r="A4" s="151"/>
+      <c r="B4" s="156"/>
+      <c r="C4" s="163" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -2355,9 +2547,9 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="143"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="151"/>
+      <c r="B5" s="156"/>
+      <c r="C5" s="164"/>
       <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
@@ -2381,9 +2573,9 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="139"/>
-      <c r="B6" s="143"/>
-      <c r="C6" s="129" t="s">
+      <c r="A6" s="151"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="163" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -2409,9 +2601,9 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="139"/>
-      <c r="B7" s="143"/>
-      <c r="C7" s="148"/>
+      <c r="A7" s="151"/>
+      <c r="B7" s="156"/>
+      <c r="C7" s="165"/>
       <c r="D7" s="15" t="s">
         <v>11</v>
       </c>
@@ -2445,8 +2637,8 @@
       <c r="U7" s="36"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
-      <c r="B8" s="144"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="34" t="s">
         <v>41</v>
       </c>
@@ -2483,11 +2675,11 @@
       <c r="U8" s="42"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="139"/>
-      <c r="B9" s="142" t="s">
+      <c r="A9" s="151"/>
+      <c r="B9" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="159" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -2513,9 +2705,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="139"/>
-      <c r="B10" s="143"/>
-      <c r="C10" s="132"/>
+      <c r="A10" s="151"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="160"/>
       <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
@@ -2539,9 +2731,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="139"/>
-      <c r="B11" s="143"/>
-      <c r="C11" s="129" t="s">
+      <c r="A11" s="151"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="163" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -2567,9 +2759,9 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
-      <c r="B12" s="143"/>
-      <c r="C12" s="130"/>
+      <c r="A12" s="151"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="164"/>
       <c r="D12" s="15" t="s">
         <v>11</v>
       </c>
@@ -2593,9 +2785,9 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="139"/>
-      <c r="B13" s="143"/>
-      <c r="C13" s="129" t="s">
+      <c r="A13" s="151"/>
+      <c r="B13" s="156"/>
+      <c r="C13" s="163" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -2621,9 +2813,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="139"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="130"/>
+      <c r="A14" s="151"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="164"/>
       <c r="D14" s="15" t="s">
         <v>11</v>
       </c>
@@ -2647,8 +2839,8 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="139"/>
-      <c r="B15" s="143"/>
+      <c r="A15" s="151"/>
+      <c r="B15" s="156"/>
       <c r="C15" s="49" t="s">
         <v>56</v>
       </c>
@@ -2675,8 +2867,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="139"/>
-      <c r="B16" s="143"/>
+      <c r="A16" s="151"/>
+      <c r="B16" s="156"/>
       <c r="C16" s="49" t="s">
         <v>37</v>
       </c>
@@ -2703,8 +2895,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="139"/>
-      <c r="B17" s="144"/>
+      <c r="A17" s="151"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="48" t="s">
         <v>43</v>
       </c>
@@ -2731,11 +2923,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="142" t="s">
+      <c r="A18" s="151"/>
+      <c r="B18" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="153" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="66" t="s">
@@ -2761,9 +2953,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="141"/>
+      <c r="A19" s="151"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="154"/>
       <c r="D19" s="67" t="s">
         <v>11</v>
       </c>
@@ -2787,8 +2979,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="139"/>
-      <c r="B20" s="144"/>
+      <c r="A20" s="151"/>
+      <c r="B20" s="157"/>
       <c r="C20" s="48" t="s">
         <v>39</v>
       </c>
@@ -2815,11 +3007,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="139"/>
-      <c r="B21" s="145" t="s">
+      <c r="A21" s="151"/>
+      <c r="B21" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="146" t="s">
+      <c r="C21" s="161" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="50" t="s">
@@ -2845,9 +3037,9 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="139"/>
-      <c r="B22" s="145"/>
-      <c r="C22" s="147"/>
+      <c r="A22" s="151"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="162"/>
       <c r="D22" s="32" t="s">
         <v>11</v>
       </c>
@@ -2871,9 +3063,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="139"/>
-      <c r="B23" s="145"/>
-      <c r="C23" s="131" t="s">
+      <c r="A23" s="151"/>
+      <c r="B23" s="158"/>
+      <c r="C23" s="159" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="31" t="s">
@@ -2899,9 +3091,9 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="136"/>
-      <c r="B24" s="145"/>
-      <c r="C24" s="132"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="158"/>
+      <c r="C24" s="160"/>
       <c r="D24" s="33" t="s">
         <v>11</v>
       </c>
@@ -2925,11 +3117,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="133" t="s">
+      <c r="A25" s="166" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="131" t="s">
+      <c r="B25" s="150"/>
+      <c r="C25" s="159" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="32" t="s">
@@ -2955,9 +3147,9 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
-      <c r="B26" s="136"/>
-      <c r="C26" s="132"/>
+      <c r="A26" s="167"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="160"/>
       <c r="D26" s="32" t="s">
         <v>11</v>
       </c>
@@ -2981,11 +3173,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="133" t="s">
+      <c r="A27" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="134"/>
-      <c r="C27" s="131" t="s">
+      <c r="B27" s="150"/>
+      <c r="C27" s="159" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="31" t="s">
@@ -3011,9 +3203,9 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="135"/>
-      <c r="B28" s="136"/>
-      <c r="C28" s="132"/>
+      <c r="A28" s="167"/>
+      <c r="B28" s="152"/>
+      <c r="C28" s="160"/>
       <c r="D28" s="33" t="s">
         <v>11</v>
       </c>
@@ -3037,10 +3229,10 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="137" t="s">
+      <c r="A29" s="148" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="138"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="48" t="s">
         <v>52</v>
       </c>
@@ -3068,6 +3260,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="A27:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A2:A24"/>
     <mergeCell ref="C18:C19"/>
@@ -3084,9 +3279,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="A27:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3113,26 +3305,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="177" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="168" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="150"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="152" t="s">
+      <c r="D1" s="169"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="171" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="153"/>
-      <c r="H1" s="154"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="173"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="159"/>
-      <c r="B2" s="128"/>
+      <c r="A2" s="178"/>
+      <c r="B2" s="144"/>
       <c r="C2" s="5" t="s">
         <v>27</v>
       </c>
@@ -3153,7 +3345,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="174" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -3179,7 +3371,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
+      <c r="A4" s="174"/>
       <c r="B4" s="6" t="s">
         <v>95</v>
       </c>
@@ -3203,7 +3395,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
+      <c r="A5" s="174"/>
       <c r="B5" s="6" t="s">
         <v>96</v>
       </c>
@@ -3227,7 +3419,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="175" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3253,7 +3445,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="157"/>
+      <c r="A7" s="176"/>
       <c r="B7" s="6" t="s">
         <v>98</v>
       </c>
@@ -3294,12 +3486,1406 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>24.711642857142898</v>
+      </c>
+      <c r="C2">
+        <v>0.44765772473266602</v>
+      </c>
+      <c r="D2">
+        <v>55.202091892640198</v>
+      </c>
+      <c r="E2" s="179">
+        <v>1.19324726915733E-87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>0.855690476190476</v>
+      </c>
+      <c r="C3">
+        <v>0.71563034264245495</v>
+      </c>
+      <c r="D3">
+        <v>1.1957157560296401</v>
+      </c>
+      <c r="E3">
+        <v>0.23414553525416801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>2.9073571428571401</v>
+      </c>
+      <c r="C4">
+        <v>1.7337709126907199</v>
+      </c>
+      <c r="D4">
+        <v>1.6768980962687201</v>
+      </c>
+      <c r="E4">
+        <v>9.6144073353563897E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5">
+        <v>-1.15644285714286</v>
+      </c>
+      <c r="C5">
+        <v>0.69350836507628699</v>
+      </c>
+      <c r="D5">
+        <v>-1.66752546238667</v>
+      </c>
+      <c r="E5">
+        <v>9.7996107301828506E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6">
+        <v>3.2773571428571402</v>
+      </c>
+      <c r="C6">
+        <v>0.65893432913388605</v>
+      </c>
+      <c r="D6">
+        <v>4.9737234773683001</v>
+      </c>
+      <c r="E6" s="179">
+        <v>2.1942601887269799E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7">
+        <v>1.6964682539682501</v>
+      </c>
+      <c r="C7">
+        <v>0.71563034264245495</v>
+      </c>
+      <c r="D7">
+        <v>2.3705929624281601</v>
+      </c>
+      <c r="E7" s="36">
+        <v>1.9339544764155302E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>0.30253333333333299</v>
+      </c>
+      <c r="C8">
+        <v>0.70623435067714502</v>
+      </c>
+      <c r="D8">
+        <v>0.42837527379298501</v>
+      </c>
+      <c r="E8">
+        <v>0.66913950250152399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9">
+        <v>6.9857142857143201E-2</v>
+      </c>
+      <c r="C9">
+        <v>1.7337709126907199</v>
+      </c>
+      <c r="D9">
+        <v>4.0292026095148203E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.96792671755255999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>0.37066666666666698</v>
+      </c>
+      <c r="C10">
+        <v>1.76558587669286</v>
+      </c>
+      <c r="D10">
+        <v>0.20993975515989399</v>
+      </c>
+      <c r="E10">
+        <v>0.83406778096080603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>-0.80789047619047305</v>
+      </c>
+      <c r="C11">
+        <v>1.0235890223173001</v>
+      </c>
+      <c r="D11">
+        <v>-0.78927231396200004</v>
+      </c>
+      <c r="E11">
+        <v>0.43149671378471999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12">
+        <v>-3.22255714285714</v>
+      </c>
+      <c r="C12">
+        <v>1.93755309986771</v>
+      </c>
+      <c r="D12">
+        <v>-1.66320971697611</v>
+      </c>
+      <c r="E12">
+        <v>9.8858548817813502E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>-3.1517389610389599</v>
+      </c>
+      <c r="C13">
+        <v>0.98478533163783699</v>
+      </c>
+      <c r="D13">
+        <v>-3.20043247983515</v>
+      </c>
+      <c r="E13" s="36">
+        <v>1.7527472953589799E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>-1.19095396825397</v>
+      </c>
+      <c r="C14">
+        <v>1.09246422287147</v>
+      </c>
+      <c r="D14">
+        <v>-1.0901537490386899</v>
+      </c>
+      <c r="E14">
+        <v>0.27781166139024399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15">
+        <v>4.4008416666666603</v>
+      </c>
+      <c r="C15">
+        <v>1.0509584962565299</v>
+      </c>
+      <c r="D15">
+        <v>4.1874552442768103</v>
+      </c>
+      <c r="E15" s="179">
+        <v>5.3828401638443797E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16">
+        <v>6.9463928571428601</v>
+      </c>
+      <c r="C16">
+        <v>2.04326861564599</v>
+      </c>
+      <c r="D16">
+        <v>3.3996474100135399</v>
+      </c>
+      <c r="E16" s="36">
+        <v>9.1443641241083402E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17">
+        <v>2.2623333333333302</v>
+      </c>
+      <c r="C17">
+        <v>1.98329463297645</v>
+      </c>
+      <c r="D17">
+        <v>1.1406945270346001</v>
+      </c>
+      <c r="E17">
+        <v>0.25624978160237499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>24.711642857142898</v>
+      </c>
+      <c r="C2">
+        <v>0.44765772473266502</v>
+      </c>
+      <c r="D2">
+        <v>55.202091892640297</v>
+      </c>
+      <c r="E2" s="179">
+        <v>1.1932472691573001E-87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>-1.15644285714286</v>
+      </c>
+      <c r="C3">
+        <v>0.69350836507628699</v>
+      </c>
+      <c r="D3">
+        <v>-1.66752546238667</v>
+      </c>
+      <c r="E3">
+        <v>9.7996107301828006E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>3.2773571428571402</v>
+      </c>
+      <c r="C4">
+        <v>0.65893432913388605</v>
+      </c>
+      <c r="D4">
+        <v>4.9737234773683001</v>
+      </c>
+      <c r="E4" s="179">
+        <v>2.1942601887269799E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>1.6964682539682501</v>
+      </c>
+      <c r="C5">
+        <v>0.71563034264245495</v>
+      </c>
+      <c r="D5">
+        <v>2.3705929624281601</v>
+      </c>
+      <c r="E5">
+        <v>1.9339544764155399E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>1.15822380952381</v>
+      </c>
+      <c r="C6">
+        <v>0.62244280684370101</v>
+      </c>
+      <c r="D6">
+        <v>1.86077145850068</v>
+      </c>
+      <c r="E6">
+        <v>6.5203883074817198E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>2.97721428571429</v>
+      </c>
+      <c r="C7">
+        <v>0.63308362561801701</v>
+      </c>
+      <c r="D7">
+        <v>4.70271882771873</v>
+      </c>
+      <c r="E7" s="179">
+        <v>6.8714024562480201E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8">
+        <v>2.9073571428571401</v>
+      </c>
+      <c r="C8">
+        <v>1.7337709126907199</v>
+      </c>
+      <c r="D8">
+        <v>1.6768980962687201</v>
+      </c>
+      <c r="E8">
+        <v>9.6144073353563994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9">
+        <v>1.22635714285714</v>
+      </c>
+      <c r="C9">
+        <v>1.7337709126907199</v>
+      </c>
+      <c r="D9">
+        <v>0.70733516976236599</v>
+      </c>
+      <c r="E9">
+        <v>0.48071831805130499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10">
+        <v>0.855690476190474</v>
+      </c>
+      <c r="C10">
+        <v>0.71563034264245495</v>
+      </c>
+      <c r="D10">
+        <v>1.1957157560296401</v>
+      </c>
+      <c r="E10">
+        <v>0.23414553525416901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11">
+        <v>-3.1517389610389599</v>
+      </c>
+      <c r="C11">
+        <v>0.98478533163783599</v>
+      </c>
+      <c r="D11">
+        <v>-3.20043247983515</v>
+      </c>
+      <c r="E11" s="36">
+        <v>1.7527472953589899E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <v>-1.19095396825397</v>
+      </c>
+      <c r="C12">
+        <v>1.09246422287147</v>
+      </c>
+      <c r="D12">
+        <v>-1.0901537490386799</v>
+      </c>
+      <c r="E12">
+        <v>0.27781166139024499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13">
+        <v>3.5929511904761902</v>
+      </c>
+      <c r="C13">
+        <v>1.0093002423000199</v>
+      </c>
+      <c r="D13">
+        <v>3.5598437807648802</v>
+      </c>
+      <c r="E13" s="36">
+        <v>5.3127104969727596E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14">
+        <v>3.7238357142857099</v>
+      </c>
+      <c r="C14">
+        <v>1.1759006445012701</v>
+      </c>
+      <c r="D14">
+        <v>3.1667945176312799</v>
+      </c>
+      <c r="E14" s="36">
+        <v>1.9509127261330499E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15">
+        <v>-3.22255714285714</v>
+      </c>
+      <c r="C15">
+        <v>1.93755309986771</v>
+      </c>
+      <c r="D15">
+        <v>-1.6632097169761</v>
+      </c>
+      <c r="E15">
+        <v>9.8858548817813696E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16">
+        <v>1.45444285714286</v>
+      </c>
+      <c r="C16">
+        <v>1.9615378710201501</v>
+      </c>
+      <c r="D16">
+        <v>0.74148089549065699</v>
+      </c>
+      <c r="E16">
+        <v>0.459838618479401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17">
+        <v>-0.80789047619047005</v>
+      </c>
+      <c r="C17">
+        <v>1.0235890223173001</v>
+      </c>
+      <c r="D17">
+        <v>-0.78927231396199704</v>
+      </c>
+      <c r="E17">
+        <v>0.43149671378472099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>24.711642857142898</v>
+      </c>
+      <c r="C2">
+        <v>0.46979987749491398</v>
+      </c>
+      <c r="D2">
+        <v>52.600360368144997</v>
+      </c>
+      <c r="E2" s="179">
+        <v>3.2469395311454599E-56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>0.85569047619046701</v>
+      </c>
+      <c r="C3">
+        <v>0.75102702071285399</v>
+      </c>
+      <c r="D3">
+        <v>1.1393604392266301</v>
+      </c>
+      <c r="E3">
+        <v>0.25860997922761902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>2.9073571428571401</v>
+      </c>
+      <c r="C4">
+        <v>1.8195271015880901</v>
+      </c>
+      <c r="D4">
+        <v>1.59786415949484</v>
+      </c>
+      <c r="E4">
+        <v>0.114779131054491</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>3.2773571428571402</v>
+      </c>
+      <c r="C5">
+        <v>0.69152669551086698</v>
+      </c>
+      <c r="D5">
+        <v>4.7393067601475396</v>
+      </c>
+      <c r="E5" s="179">
+        <v>1.15885934666249E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6">
+        <v>1.6964682539682501</v>
+      </c>
+      <c r="C6">
+        <v>0.75102702071285399</v>
+      </c>
+      <c r="D6">
+        <v>2.2588644711584598</v>
+      </c>
+      <c r="E6">
+        <v>2.71511458286758E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7">
+        <v>0.30253333333334298</v>
+      </c>
+      <c r="C7">
+        <v>0.74116628196009005</v>
+      </c>
+      <c r="D7">
+        <v>0.40818550532717501</v>
+      </c>
+      <c r="E7">
+        <v>0.68443905764368795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8">
+        <v>6.9857142857144602E-2</v>
+      </c>
+      <c r="C8">
+        <v>1.8195271015880901</v>
+      </c>
+      <c r="D8">
+        <v>3.8393021349433697E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.96948849458932496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9">
+        <v>0.37066666666667503</v>
+      </c>
+      <c r="C9">
+        <v>1.8529157049002201</v>
+      </c>
+      <c r="D9">
+        <v>0.200045077974356</v>
+      </c>
+      <c r="E9">
+        <v>0.84205127381507106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12">
+        <v>24.711642857142898</v>
+      </c>
+      <c r="C12">
+        <v>0.46979987749491398</v>
+      </c>
+      <c r="D12">
+        <v>52.600360368144997</v>
+      </c>
+      <c r="E12" s="179">
+        <v>3.2469395311454599E-56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13">
+        <v>3.2773571428571402</v>
+      </c>
+      <c r="C13">
+        <v>0.69152669551086599</v>
+      </c>
+      <c r="D13">
+        <v>4.7393067601475503</v>
+      </c>
+      <c r="E13" s="179">
+        <v>1.15885934666249E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14">
+        <v>1.6964682539682501</v>
+      </c>
+      <c r="C14">
+        <v>0.75102702071285399</v>
+      </c>
+      <c r="D14">
+        <v>2.2588644711584598</v>
+      </c>
+      <c r="E14" s="36">
+        <v>2.71511458286758E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15">
+        <v>1.15822380952381</v>
+      </c>
+      <c r="C15">
+        <v>0.65323022087330795</v>
+      </c>
+      <c r="D15">
+        <v>1.77307138052396</v>
+      </c>
+      <c r="E15">
+        <v>8.0761947923766106E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16">
+        <v>2.9772142857142798</v>
+      </c>
+      <c r="C16">
+        <v>0.66439735835452596</v>
+      </c>
+      <c r="D16">
+        <v>4.4810748391411099</v>
+      </c>
+      <c r="E16" s="179">
+        <v>2.9724948876506599E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17">
+        <v>2.9073571428571401</v>
+      </c>
+      <c r="C17">
+        <v>1.8195271015880901</v>
+      </c>
+      <c r="D17">
+        <v>1.5978641594948499</v>
+      </c>
+      <c r="E17">
+        <v>0.11477913105449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18">
+        <v>1.22635714285714</v>
+      </c>
+      <c r="C18">
+        <v>1.8195271015880901</v>
+      </c>
+      <c r="D18">
+        <v>0.67399773368958005</v>
+      </c>
+      <c r="E18">
+        <v>0.50263153148704598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19">
+        <v>0.85569047619046601</v>
+      </c>
+      <c r="C19">
+        <v>0.75102702071285399</v>
+      </c>
+      <c r="D19">
+        <v>1.1393604392266301</v>
+      </c>
+      <c r="E19">
+        <v>0.25860997922761902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>23.555199999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.491365698764681</v>
+      </c>
+      <c r="D2">
+        <v>47.938226170892698</v>
+      </c>
+      <c r="E2" s="179">
+        <v>3.70900312056121E-47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>-1.3615333333333399</v>
+      </c>
+      <c r="C3">
+        <v>1.0228592684223501</v>
+      </c>
+      <c r="D3">
+        <v>-1.33110524132352</v>
+      </c>
+      <c r="E3">
+        <v>0.188548388505347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>-0.31520000000000098</v>
+      </c>
+      <c r="C4">
+        <v>0.80239682605304996</v>
+      </c>
+      <c r="D4">
+        <v>-0.39282308923186299</v>
+      </c>
+      <c r="E4">
+        <v>0.69594151418921801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>0.12561818181818099</v>
+      </c>
+      <c r="C5">
+        <v>0.67891927812935704</v>
+      </c>
+      <c r="D5">
+        <v>0.185026682648194</v>
+      </c>
+      <c r="E5">
+        <v>0.85387659902313096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6">
+        <v>0.50551428571428503</v>
+      </c>
+      <c r="C6">
+        <v>0.76573813583295902</v>
+      </c>
+      <c r="D6">
+        <v>0.66016600461513397</v>
+      </c>
+      <c r="E6">
+        <v>0.51185364575692105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7">
+        <v>-1.7472000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.6296756576532401</v>
+      </c>
+      <c r="D7">
+        <v>-1.0721151732216401</v>
+      </c>
+      <c r="E7">
+        <v>0.28826696891922798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>6.1127083333333303</v>
+      </c>
+      <c r="C8">
+        <v>1.0519511136351101</v>
+      </c>
+      <c r="D8">
+        <v>5.8108292810398297</v>
+      </c>
+      <c r="E8" s="179">
+        <v>3.0812815812629402E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9">
+        <v>7.0162500000000003</v>
+      </c>
+      <c r="C9">
+        <v>1.0029960325663101</v>
+      </c>
+      <c r="D9">
+        <v>6.9952918777234796</v>
+      </c>
+      <c r="E9" s="179">
+        <v>3.5233981084583199E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>4.04233333333333</v>
+      </c>
+      <c r="C10">
+        <v>1.13476047380935</v>
+      </c>
+      <c r="D10">
+        <v>3.5622789360677798</v>
+      </c>
+      <c r="E10" s="36">
+        <v>7.5935298199140305E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>1.40933333333333</v>
+      </c>
+      <c r="C11">
+        <v>1.0120731047548901</v>
+      </c>
+      <c r="D11">
+        <v>1.39252127806979</v>
+      </c>
+      <c r="E11">
+        <v>0.169269338192581</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12">
+        <v>3.4063333333333401</v>
+      </c>
+      <c r="C12">
+        <v>1.7942138479846901</v>
+      </c>
+      <c r="D12">
+        <v>1.89851022338247</v>
+      </c>
+      <c r="E12">
+        <v>6.2786331054812405E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13">
+        <v>2.70333333333333</v>
+      </c>
+      <c r="C13">
+        <v>1.7942138479846901</v>
+      </c>
+      <c r="D13">
+        <v>1.50669516700575</v>
+      </c>
+      <c r="E13">
+        <v>0.13750947083154899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16">
+        <v>23.555199999999999</v>
+      </c>
+      <c r="C16">
+        <v>0.491365698764681</v>
+      </c>
+      <c r="D16">
+        <v>47.938226170892698</v>
+      </c>
+      <c r="E16" s="179">
+        <v>3.70900312056121E-47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17">
+        <v>0.12561818181818199</v>
+      </c>
+      <c r="C17">
+        <v>0.67891927812935704</v>
+      </c>
+      <c r="D17">
+        <v>0.185026682648194</v>
+      </c>
+      <c r="E17">
+        <v>0.85387659902312996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <v>0.50551428571428603</v>
+      </c>
+      <c r="C18">
+        <v>0.76573813583296002</v>
+      </c>
+      <c r="D18">
+        <v>0.66016600461513497</v>
+      </c>
+      <c r="E18">
+        <v>0.51185364575692005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19">
+        <v>-1.7472000000000001</v>
+      </c>
+      <c r="C19">
+        <v>1.6296756576532401</v>
+      </c>
+      <c r="D19">
+        <v>-1.0721151732216401</v>
+      </c>
+      <c r="E19">
+        <v>0.28826696891922798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20">
+        <v>4.7511749999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.73704854814702103</v>
+      </c>
+      <c r="D20">
+        <v>6.4462171616031299</v>
+      </c>
+      <c r="E20" s="179">
+        <v>2.83192416946778E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21">
+        <v>6.7010500000000004</v>
+      </c>
+      <c r="C21">
+        <v>0.91926104819510401</v>
+      </c>
+      <c r="D21">
+        <v>7.2896050726363102</v>
+      </c>
+      <c r="E21" s="179">
+        <v>1.1495244749831801E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22">
+        <v>-0.31519999999999998</v>
+      </c>
+      <c r="C22">
+        <v>0.80239682605304996</v>
+      </c>
+      <c r="D22">
+        <v>-0.39282308923186199</v>
+      </c>
+      <c r="E22">
+        <v>0.69594151418921901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>2.6808000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.85107035535701103</v>
+      </c>
+      <c r="D23">
+        <v>3.1499158478800999</v>
+      </c>
+      <c r="E23" s="36">
+        <v>2.62029039670943E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24">
+        <v>4.7799999999998399E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.67891927812935704</v>
+      </c>
+      <c r="D24">
+        <v>7.0406013704166603E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.94412133382831998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25">
+        <v>2.0448</v>
+      </c>
+      <c r="C25">
+        <v>1.6296756576532401</v>
+      </c>
+      <c r="D25">
+        <v>1.25472819723192</v>
+      </c>
+      <c r="E25">
+        <v>0.21478892950204201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26">
+        <v>1.3418000000000001</v>
+      </c>
+      <c r="C26">
+        <v>1.6296756576532401</v>
+      </c>
+      <c r="D26">
+        <v>0.82335401753021797</v>
+      </c>
+      <c r="E26">
+        <v>0.41379937310566001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27">
+        <v>-1.3615333333333299</v>
+      </c>
+      <c r="C27">
+        <v>1.0228592684223501</v>
+      </c>
+      <c r="D27">
+        <v>-1.33110524132352</v>
+      </c>
+      <c r="E27">
+        <v>0.188548388505348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding model results and starting to format
</commit_message>
<xml_diff>
--- a/doc/MainTables.xlsx
+++ b/doc/MainTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7005" windowHeight="4575" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Table1 Strain.Info" sheetId="3" r:id="rId1"/>
@@ -21,14 +21,33 @@
     <sheet name="MLH1_M3" sheetId="7" r:id="rId7"/>
     <sheet name="MLH1_M4.M5_female" sheetId="8" r:id="rId8"/>
     <sheet name="MLH1_M4.M5_male" sheetId="9" r:id="rId9"/>
+    <sheet name="total sc" sheetId="10" r:id="rId10"/>
+    <sheet name="short SC" sheetId="13" r:id="rId11"/>
+    <sheet name="nrm F1 pos" sheetId="11" r:id="rId12"/>
+    <sheet name="Q1 IFD" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="ABS.IFD_Q1_M1" localSheetId="12">'Q1 IFD'!$A$2:$E$3</definedName>
+    <definedName name="ABS.IFD_Q1_M2" localSheetId="12">'Q1 IFD'!$A$6:$E$20</definedName>
+    <definedName name="ABS.IFD_Q1_M3" localSheetId="12">'Q1 IFD'!$A$24:$E$39</definedName>
     <definedName name="MLH1_M2_glm" localSheetId="5">MLH1_M2!$A$1:$E$17</definedName>
     <definedName name="MLH1_M3_glm" localSheetId="6">MLH1_M3!$A$1:$E$17</definedName>
     <definedName name="MLH1_M4_female_glm" localSheetId="7">MLH1_M4.M5_female!$A$1:$E$9</definedName>
     <definedName name="MLH1_M4_male_glm" localSheetId="8">MLH1_M4.M5_male!$A$1:$E$13</definedName>
     <definedName name="MLH1_M5_female_glm" localSheetId="7">MLH1_M4.M5_female!$A$11:$E$19</definedName>
     <definedName name="MLH1_M5_male_glm" localSheetId="8">MLH1_M4.M5_male!$A$15:$E$27</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M1" localSheetId="11">'nrm F1 pos'!$A$1:$E$2</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M2" localSheetId="11">'nrm F1 pos'!$A$7:$E$21</definedName>
+    <definedName name="Nrm1CO_Pos_Q1_M3" localSheetId="11">'nrm F1 pos'!$A$25:$E$39</definedName>
+    <definedName name="PER.IFD_Q1_M1" localSheetId="12">'Q1 IFD'!#REF!</definedName>
+    <definedName name="PER.IFD_Q1_M2" localSheetId="12">'Q1 IFD'!$H$5:$L$20</definedName>
+    <definedName name="PER.IFD_Q1_M3" localSheetId="12">'Q1 IFD'!$H$24:$L$39</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="10">'short SC'!$A$1:$E$2</definedName>
+    <definedName name="ShortSC_Q1_M1" localSheetId="9">'total sc'!$A$2:$E$3</definedName>
+    <definedName name="ShortSC_Q1_M2" localSheetId="10">'short SC'!$A$6:$E$19</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="10">'short SC'!$A$22:$E$35</definedName>
+    <definedName name="ShortSC_Q1_M3" localSheetId="9">'total sc'!$A$24:$E$37</definedName>
+    <definedName name="TotalSC_Q1_M2" localSheetId="9">'total sc'!$A$6:$E$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,8 +60,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="MLH1_M2_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M2_glm.csv" comma="1">
+  <connection id="1" name="ABS.IFD_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ABS.IFD_Q1_M1.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -52,8 +71,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="MLH1_M3_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M3_glm.csv" tab="0" comma="1">
+  <connection id="2" name="ABS.IFD_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ABS.IFD_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -63,8 +82,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="MLH1_M4_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_female_glm.csv" comma="1">
+  <connection id="3" name="ABS.IFD_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ABS.IFD_Q1_M3.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -74,8 +93,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="MLH1_M4_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_male_glm.csv" tab="0" comma="1">
+  <connection id="4" name="MLH1_M2_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M2_glm.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -85,8 +104,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="MLH1_M5_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_female_glm.csv" comma="1">
+  <connection id="5" name="MLH1_M3_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M3_glm.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -96,8 +115,162 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="MLH1_M5_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" name="MLH1_M4_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_female_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="MLH1_M4_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M4_male_glm.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="MLH1_M5_female_glm" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_female_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="MLH1_M5_male_glm" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\MLH1_M5_male_glm.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" name="Nrm1CO_Pos_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M1.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" name="Nrm1CO_Pos_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M2.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" name="Nrm1CO_Pos_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\Nrm1CO_Pos_Q1_M3.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="13" name="PER.IFD_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M2.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="14" name="PER.IFD_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\PER.IFD_Q1_M3.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="15" name="ShortSC_Q1_M1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="16" name="ShortSC_Q1_M11" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M1.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="17" name="ShortSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M2.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="18" name="ShortSC_Q1_M3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="19" name="ShortSC_Q1_M31" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\ShortSC_Q1_M3.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="20" name="TotalSC_Q1_M2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\April\Documents\MLH1repo\TotalSC_Q1_M2.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -111,7 +284,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="162">
   <si>
     <t>Species</t>
   </si>
@@ -645,6 +818,63 @@
   </si>
   <si>
     <t>strainCZECH</t>
+  </si>
+  <si>
+    <t>sub.sp</t>
+  </si>
+  <si>
+    <t>sex.results</t>
+  </si>
+  <si>
+    <t>interaction.pval</t>
+  </si>
+  <si>
+    <t>rand.pval</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>strainG:sexmale</t>
+  </si>
+  <si>
+    <t>strainLEW:sexmale</t>
+  </si>
+  <si>
+    <t>strainPWD:sexmale</t>
+  </si>
+  <si>
+    <t>strainSKIVE:sexmale</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>strainKAZ:sexmale</t>
+  </si>
+  <si>
+    <t>strainMSM:sexmale</t>
+  </si>
+  <si>
+    <t>M1_ABS_IFD</t>
+  </si>
+  <si>
+    <t>M1_PER_IFD</t>
+  </si>
+  <si>
+    <t>M2_ABS_IFD</t>
+  </si>
+  <si>
+    <t>M2_PER_IFD</t>
+  </si>
+  <si>
+    <t>M3_ABS_IFD</t>
+  </si>
+  <si>
+    <t>M3_PER_IFD</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1510,6 +1740,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1530,27 +1761,83 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M2_glm" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M2_glm" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M3" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Nrm1CO_Pos_Q1_M1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M3" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PER.IFD_Q1_M2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M3_glm" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M3_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABS.IFD_Q1_M1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_female_glm" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_female_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M5_male_glm" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MLH1_M4_male_glm" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M3" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TotalSC_Q1_M2" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ShortSC_Q1_M1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2150,6 +2437,2788 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.131713810169865</v>
+      </c>
+      <c r="B3" s="179">
+        <v>1.27468066684173E-11</v>
+      </c>
+      <c r="C3">
+        <v>3.3477300526601202E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.2046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7">
+        <v>1683.2049671151101</v>
+      </c>
+      <c r="C7">
+        <v>61.661944758599297</v>
+      </c>
+      <c r="D7">
+        <v>27.297305878118198</v>
+      </c>
+      <c r="E7" s="179">
+        <v>1.7892479246577E-60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <v>415.17246918414997</v>
+      </c>
+      <c r="C8">
+        <v>193.65432080005499</v>
+      </c>
+      <c r="D8">
+        <v>2.14388435780273</v>
+      </c>
+      <c r="E8">
+        <v>3.3632589894028099E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9">
+        <v>157.89689533670699</v>
+      </c>
+      <c r="C9">
+        <v>90.063034890459406</v>
+      </c>
+      <c r="D9">
+        <v>1.7531820410976799</v>
+      </c>
+      <c r="E9">
+        <v>8.1586699628115697E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>598.57741472631096</v>
+      </c>
+      <c r="C10">
+        <v>91.755910036897504</v>
+      </c>
+      <c r="D10">
+        <v>6.5235843062927099</v>
+      </c>
+      <c r="E10" s="179">
+        <v>9.6230751267210195E-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>251.706957540693</v>
+      </c>
+      <c r="C11">
+        <v>101.32091425176699</v>
+      </c>
+      <c r="D11">
+        <v>2.48425470101109</v>
+      </c>
+      <c r="E11">
+        <v>1.4066937527411999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>-212.18960320394601</v>
+      </c>
+      <c r="C12">
+        <v>193.108163693324</v>
+      </c>
+      <c r="D12">
+        <v>-1.0988121845585199</v>
+      </c>
+      <c r="E12">
+        <v>0.27358741112094198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>-135.35009568113099</v>
+      </c>
+      <c r="C13">
+        <v>223.29158317460499</v>
+      </c>
+      <c r="D13">
+        <v>-0.60615852042793905</v>
+      </c>
+      <c r="E13">
+        <v>0.54531366039367501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14">
+        <v>-185.42600443094901</v>
+      </c>
+      <c r="C14">
+        <v>162.843101878277</v>
+      </c>
+      <c r="D14">
+        <v>-1.1386789019135299</v>
+      </c>
+      <c r="E14">
+        <v>0.25662856320217597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15">
+        <v>-331.522473509669</v>
+      </c>
+      <c r="C15">
+        <v>93.671218361957898</v>
+      </c>
+      <c r="D15">
+        <v>-3.53921385145886</v>
+      </c>
+      <c r="E15">
+        <v>5.3276127042585801E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16">
+        <v>-99.688296122924996</v>
+      </c>
+      <c r="C16">
+        <v>144.666248901373</v>
+      </c>
+      <c r="D16">
+        <v>-0.68909159448026003</v>
+      </c>
+      <c r="E16">
+        <v>0.49181616591767302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17">
+        <v>170.42009642077301</v>
+      </c>
+      <c r="C17">
+        <v>142.35651258534099</v>
+      </c>
+      <c r="D17">
+        <v>1.1971359323558</v>
+      </c>
+      <c r="E17">
+        <v>0.233117271852015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18">
+        <v>-481.68135090133802</v>
+      </c>
+      <c r="C18">
+        <v>130.315812918425</v>
+      </c>
+      <c r="D18">
+        <v>-3.6962617207695301</v>
+      </c>
+      <c r="E18">
+        <v>3.04881880909094E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <v>-177.698708000392</v>
+      </c>
+      <c r="C19">
+        <v>147.31517782026501</v>
+      </c>
+      <c r="D19">
+        <v>-1.20624847099731</v>
+      </c>
+      <c r="E19">
+        <v>0.22959584868837499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20">
+        <v>123.373633340476</v>
+      </c>
+      <c r="C20">
+        <v>154.35236980824601</v>
+      </c>
+      <c r="D20">
+        <v>0.79929860159416</v>
+      </c>
+      <c r="E20">
+        <v>0.42536455524917899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21">
+        <v>-108.85532312591199</v>
+      </c>
+      <c r="C21">
+        <v>197.70241288601599</v>
+      </c>
+      <c r="D21">
+        <v>-0.55060189472079102</v>
+      </c>
+      <c r="E21">
+        <v>0.58271491548015997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25">
+        <v>73.886333333333397</v>
+      </c>
+      <c r="C25">
+        <v>4.6370848367779303</v>
+      </c>
+      <c r="D25">
+        <v>15.933789424623299</v>
+      </c>
+      <c r="E25" s="179">
+        <v>1.1433738135208399E-18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26">
+        <v>7.9648333333333303</v>
+      </c>
+      <c r="C26">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D26">
+        <v>1.4024455909770699</v>
+      </c>
+      <c r="E26">
+        <v>0.168692554978048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27">
+        <v>9.1664999999999992</v>
+      </c>
+      <c r="C27">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D27">
+        <v>1.61403471631857</v>
+      </c>
+      <c r="E27">
+        <v>0.11458306791363899</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28">
+        <v>1.8291666666666699</v>
+      </c>
+      <c r="C28">
+        <v>5.4374639495153598</v>
+      </c>
+      <c r="D28">
+        <v>0.33640069776089299</v>
+      </c>
+      <c r="E28">
+        <v>0.738372129010606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29">
+        <v>1.7246666666666599</v>
+      </c>
+      <c r="C29">
+        <v>6.5578282660459797</v>
+      </c>
+      <c r="D29">
+        <v>0.262993569928684</v>
+      </c>
+      <c r="E29">
+        <v>0.79393998062023396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30">
+        <v>-7.0003333333333302</v>
+      </c>
+      <c r="C30">
+        <v>6.1342866432114702</v>
+      </c>
+      <c r="D30">
+        <v>-1.1411813207457899</v>
+      </c>
+      <c r="E30">
+        <v>0.26075352062797402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31">
+        <v>6.8969166666666704</v>
+      </c>
+      <c r="C31">
+        <v>6.1342866432114702</v>
+      </c>
+      <c r="D31">
+        <v>1.1243225280806199</v>
+      </c>
+      <c r="E31">
+        <v>0.26774893215888101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32">
+        <v>-24.321833333333299</v>
+      </c>
+      <c r="C32">
+        <v>7.3318748938241898</v>
+      </c>
+      <c r="D32">
+        <v>-3.3172733694379</v>
+      </c>
+      <c r="E32">
+        <v>1.9751870895198102E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33">
+        <v>-0.91458333333333697</v>
+      </c>
+      <c r="C33">
+        <v>8.9796761738959194</v>
+      </c>
+      <c r="D33">
+        <v>-0.101850369169441</v>
+      </c>
+      <c r="E33">
+        <v>0.91939731100514999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34">
+        <v>-3.2309999999999999</v>
+      </c>
+      <c r="C34">
+        <v>9.8367423990689709</v>
+      </c>
+      <c r="D34">
+        <v>-0.32846239831448798</v>
+      </c>
+      <c r="E34">
+        <v>0.74431922941371897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35">
+        <v>8.6726666666666592</v>
+      </c>
+      <c r="C35">
+        <v>9.1281106293125394</v>
+      </c>
+      <c r="D35">
+        <v>0.95010534149494896</v>
+      </c>
+      <c r="E35">
+        <v>0.34790974056242102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36">
+        <v>16.125333333333302</v>
+      </c>
+      <c r="C36">
+        <v>9.2741696735558605</v>
+      </c>
+      <c r="D36">
+        <v>1.73873607028268</v>
+      </c>
+      <c r="E36">
+        <v>8.9970840555934295E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37">
+        <v>0.94525000000000203</v>
+      </c>
+      <c r="C37">
+        <v>9.5595952884927105</v>
+      </c>
+      <c r="D37">
+        <v>9.8879708970299102E-2</v>
+      </c>
+      <c r="E37">
+        <v>0.92174027757396004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.131713810169865</v>
+      </c>
+      <c r="B3" s="179">
+        <v>1.27468066684173E-11</v>
+      </c>
+      <c r="C3">
+        <v>3.3477300526601202E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.2046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7">
+        <v>73.886333333333397</v>
+      </c>
+      <c r="C7">
+        <v>4.6370848367779303</v>
+      </c>
+      <c r="D7">
+        <v>15.933789424623299</v>
+      </c>
+      <c r="E7" s="179">
+        <v>1.1433738135208399E-18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <v>6.8969166666666704</v>
+      </c>
+      <c r="C8">
+        <v>6.1342866432114702</v>
+      </c>
+      <c r="D8">
+        <v>1.1243225280806199</v>
+      </c>
+      <c r="E8">
+        <v>0.26774893215888101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9">
+        <v>1.7246666666666599</v>
+      </c>
+      <c r="C9">
+        <v>6.5578282660459797</v>
+      </c>
+      <c r="D9">
+        <v>0.262993569928684</v>
+      </c>
+      <c r="E9">
+        <v>0.79393998062023496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>7.9648333333333303</v>
+      </c>
+      <c r="C10">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D10">
+        <v>1.4024455909770699</v>
+      </c>
+      <c r="E10">
+        <v>0.168692554978049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>9.1664999999999903</v>
+      </c>
+      <c r="C11">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D11">
+        <v>1.61403471631857</v>
+      </c>
+      <c r="E11">
+        <v>0.11458306791363899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>-5.0677500000000002</v>
+      </c>
+      <c r="C12">
+        <v>4.9183711995344801</v>
+      </c>
+      <c r="D12">
+        <v>-1.03037159954085</v>
+      </c>
+      <c r="E12">
+        <v>0.30918353389573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>-13.89725</v>
+      </c>
+      <c r="C13">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D13">
+        <v>-2.4470238325814901</v>
+      </c>
+      <c r="E13">
+        <v>1.9012517428052701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14">
+        <v>-24.321833333333299</v>
+      </c>
+      <c r="C14">
+        <v>7.3318748938241898</v>
+      </c>
+      <c r="D14">
+        <v>-3.3172733694379</v>
+      </c>
+      <c r="E14">
+        <v>1.9751870895198002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15">
+        <v>0.94524999999999404</v>
+      </c>
+      <c r="C15">
+        <v>9.5595952884927105</v>
+      </c>
+      <c r="D15">
+        <v>9.8879708970298297E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.92174027757396104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16">
+        <v>-0.91458333333332797</v>
+      </c>
+      <c r="C16">
+        <v>8.9796761738959301</v>
+      </c>
+      <c r="D16">
+        <v>-0.10185036916944</v>
+      </c>
+      <c r="E16">
+        <v>0.91939731100515099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>-3.2309999999999901</v>
+      </c>
+      <c r="C17">
+        <v>9.8367423990689602</v>
+      </c>
+      <c r="D17">
+        <v>-0.32846239831448698</v>
+      </c>
+      <c r="E17">
+        <v>0.74431922941371997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18">
+        <v>7.7274166666666799</v>
+      </c>
+      <c r="C18">
+        <v>8.1972853325574704</v>
+      </c>
+      <c r="D18">
+        <v>0.94267996698558298</v>
+      </c>
+      <c r="E18">
+        <v>0.35164786709389201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19">
+        <v>15.1800833333333</v>
+      </c>
+      <c r="C19">
+        <v>8.3596235738396896</v>
+      </c>
+      <c r="D19">
+        <v>1.81588120556497</v>
+      </c>
+      <c r="E19">
+        <v>7.70822265499745E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23">
+        <v>73.886333333333397</v>
+      </c>
+      <c r="C23">
+        <v>4.6370848367779303</v>
+      </c>
+      <c r="D23">
+        <v>15.933789424623299</v>
+      </c>
+      <c r="E23" s="179">
+        <v>1.1433738135208399E-18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24">
+        <v>7.9648333333333303</v>
+      </c>
+      <c r="C24">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D24">
+        <v>1.4024455909770699</v>
+      </c>
+      <c r="E24">
+        <v>0.168692554978048</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25">
+        <v>9.1664999999999992</v>
+      </c>
+      <c r="C25">
+        <v>5.67924587205147</v>
+      </c>
+      <c r="D25">
+        <v>1.61403471631857</v>
+      </c>
+      <c r="E25">
+        <v>0.11458306791363899</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26">
+        <v>1.8291666666666699</v>
+      </c>
+      <c r="C26">
+        <v>5.4374639495153598</v>
+      </c>
+      <c r="D26">
+        <v>0.33640069776089299</v>
+      </c>
+      <c r="E26">
+        <v>0.738372129010606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27">
+        <v>1.7246666666666599</v>
+      </c>
+      <c r="C27">
+        <v>6.5578282660459797</v>
+      </c>
+      <c r="D27">
+        <v>0.262993569928684</v>
+      </c>
+      <c r="E27">
+        <v>0.79393998062023396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28">
+        <v>-7.0003333333333302</v>
+      </c>
+      <c r="C28">
+        <v>6.1342866432114702</v>
+      </c>
+      <c r="D28">
+        <v>-1.1411813207457899</v>
+      </c>
+      <c r="E28">
+        <v>0.26075352062797402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29">
+        <v>6.8969166666666704</v>
+      </c>
+      <c r="C29">
+        <v>6.1342866432114702</v>
+      </c>
+      <c r="D29">
+        <v>1.1243225280806199</v>
+      </c>
+      <c r="E29">
+        <v>0.26774893215888101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30">
+        <v>-24.321833333333299</v>
+      </c>
+      <c r="C30">
+        <v>7.3318748938241898</v>
+      </c>
+      <c r="D30">
+        <v>-3.3172733694379</v>
+      </c>
+      <c r="E30">
+        <v>1.9751870895198102E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31">
+        <v>-0.91458333333333697</v>
+      </c>
+      <c r="C31">
+        <v>8.9796761738959194</v>
+      </c>
+      <c r="D31">
+        <v>-0.101850369169441</v>
+      </c>
+      <c r="E31">
+        <v>0.91939731100514999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32">
+        <v>-3.2309999999999999</v>
+      </c>
+      <c r="C32">
+        <v>9.8367423990689709</v>
+      </c>
+      <c r="D32">
+        <v>-0.32846239831448798</v>
+      </c>
+      <c r="E32">
+        <v>0.74431922941371897</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33">
+        <v>8.6726666666666592</v>
+      </c>
+      <c r="C33">
+        <v>9.1281106293125394</v>
+      </c>
+      <c r="D33">
+        <v>0.95010534149494896</v>
+      </c>
+      <c r="E33">
+        <v>0.34790974056242102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34">
+        <v>16.125333333333302</v>
+      </c>
+      <c r="C34">
+        <v>9.2741696735558605</v>
+      </c>
+      <c r="D34">
+        <v>1.73873607028268</v>
+      </c>
+      <c r="E34">
+        <v>8.9970840555934295E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35">
+        <v>0.94525000000000203</v>
+      </c>
+      <c r="C35">
+        <v>9.5595952884927105</v>
+      </c>
+      <c r="D35">
+        <v>9.8879708970299102E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.92174027757396004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.13695466066482401</v>
+      </c>
+      <c r="B4" s="179">
+        <v>7.7919070026701195E-26</v>
+      </c>
+      <c r="C4">
+        <v>6.2459740856182402E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
+        <v>0.59048073530728595</v>
+      </c>
+      <c r="C8">
+        <v>1.8102503511149001E-2</v>
+      </c>
+      <c r="D8">
+        <v>32.618733367106898</v>
+      </c>
+      <c r="E8" s="179">
+        <v>9.6065492446920407E-41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9">
+        <v>-4.3414450365285399E-2</v>
+      </c>
+      <c r="C9">
+        <v>2.2898056978570398E-2</v>
+      </c>
+      <c r="D9">
+        <v>-1.8959883978765399</v>
+      </c>
+      <c r="E9">
+        <v>6.2624212596158496E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10">
+        <v>-1.5660624783316101E-2</v>
+      </c>
+      <c r="C10">
+        <v>2.39473611990869E-2</v>
+      </c>
+      <c r="D10">
+        <v>-0.65396035300595901</v>
+      </c>
+      <c r="E10">
+        <v>0.51555571392572397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11">
+        <v>-3.8636093389946398E-2</v>
+      </c>
+      <c r="C11">
+        <v>2.2170948334627998E-2</v>
+      </c>
+      <c r="D11">
+        <v>-1.7426450509382201</v>
+      </c>
+      <c r="E11">
+        <v>8.6353801163340502E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12">
+        <v>-5.0773202365037698E-2</v>
+      </c>
+      <c r="C12">
+        <v>2.1227066940238098E-2</v>
+      </c>
+      <c r="D12">
+        <v>-2.39190852452592</v>
+      </c>
+      <c r="E12">
+        <v>1.9807072865664299E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13">
+        <v>2.7795920147631801E-2</v>
+      </c>
+      <c r="C13">
+        <v>1.6911335844131702E-2</v>
+      </c>
+      <c r="D13">
+        <v>1.64362652387848</v>
+      </c>
+      <c r="E13">
+        <v>0.10531550569824601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>3.0113873032104499E-2</v>
+      </c>
+      <c r="C14">
+        <v>2.10332083870024E-2</v>
+      </c>
+      <c r="D14">
+        <v>1.43172988533283</v>
+      </c>
+      <c r="E14">
+        <v>0.15724321407641101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15">
+        <v>0.14163874710836799</v>
+      </c>
+      <c r="C15">
+        <v>2.2898056978570499E-2</v>
+      </c>
+      <c r="D15">
+        <v>6.1856229653425601</v>
+      </c>
+      <c r="E15" s="179">
+        <v>5.3914955337116597E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16">
+        <v>-9.4059295797303093E-3</v>
+      </c>
+      <c r="C16">
+        <v>3.2382742731086198E-2</v>
+      </c>
+      <c r="D16">
+        <v>-0.29046117735731403</v>
+      </c>
+      <c r="E16">
+        <v>0.77243279892205097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17">
+        <v>1.4852022655273399E-2</v>
+      </c>
+      <c r="C17">
+        <v>3.55196767789204E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.41813507334862698</v>
+      </c>
+      <c r="E17">
+        <v>0.67729310091406503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18">
+        <v>-2.3912958275121202E-2</v>
+      </c>
+      <c r="C18">
+        <v>2.82383582124828E-2</v>
+      </c>
+      <c r="D18">
+        <v>-0.84682537473267305</v>
+      </c>
+      <c r="E18">
+        <v>0.40034939026264199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <v>1.1075393518199601E-2</v>
+      </c>
+      <c r="C19">
+        <v>2.9048737165851799E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.38126936310399301</v>
+      </c>
+      <c r="E19">
+        <v>0.70430684245473096</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20">
+        <v>-3.9870966273212502E-2</v>
+      </c>
+      <c r="C20">
+        <v>2.8466019978684601E-2</v>
+      </c>
+      <c r="D20">
+        <v>-1.4006512432390601</v>
+      </c>
+      <c r="E20">
+        <v>0.166303497895846</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21">
+        <v>-2.94376464728115E-2</v>
+      </c>
+      <c r="C21">
+        <v>3.0560543272458499E-2</v>
+      </c>
+      <c r="D21">
+        <v>-0.96325664797134103</v>
+      </c>
+      <c r="E21">
+        <v>0.33916078636810099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26">
+        <v>0.59048073530728595</v>
+      </c>
+      <c r="C26">
+        <v>1.8102503511149001E-2</v>
+      </c>
+      <c r="D26">
+        <v>32.618733367106898</v>
+      </c>
+      <c r="E26" s="179">
+        <v>9.6065492446924506E-41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27">
+        <v>-3.8636093389946398E-2</v>
+      </c>
+      <c r="C27">
+        <v>2.2170948334627998E-2</v>
+      </c>
+      <c r="D27">
+        <v>-1.7426450509382201</v>
+      </c>
+      <c r="E27">
+        <v>8.6353801163340405E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28">
+        <v>-5.0773202365037698E-2</v>
+      </c>
+      <c r="C28">
+        <v>2.1227066940238098E-2</v>
+      </c>
+      <c r="D28">
+        <v>-2.39190852452592</v>
+      </c>
+      <c r="E28">
+        <v>1.9807072865664299E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29">
+        <v>-1.5618530217653699E-2</v>
+      </c>
+      <c r="C29">
+        <v>2.0422378249887501E-2</v>
+      </c>
+      <c r="D29">
+        <v>-0.76477528848725995</v>
+      </c>
+      <c r="E29">
+        <v>0.447306581419119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30">
+        <v>-1.5660624783316101E-2</v>
+      </c>
+      <c r="C30">
+        <v>2.39473611990869E-2</v>
+      </c>
+      <c r="D30">
+        <v>-0.65396035300595901</v>
+      </c>
+      <c r="E30">
+        <v>0.51555571392572397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31">
+        <v>-1.3300577333180999E-2</v>
+      </c>
+      <c r="C31">
+        <v>2.39473611990869E-2</v>
+      </c>
+      <c r="D31">
+        <v>-0.55540889130148097</v>
+      </c>
+      <c r="E31">
+        <v>0.58061361042745896</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <v>-4.3414450365285497E-2</v>
+      </c>
+      <c r="C32">
+        <v>2.2898056978570499E-2</v>
+      </c>
+      <c r="D32">
+        <v>-1.8959883978765399</v>
+      </c>
+      <c r="E32">
+        <v>6.2624212596158704E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33">
+        <v>0.14163874710836799</v>
+      </c>
+      <c r="C33">
+        <v>2.2898056978570499E-2</v>
+      </c>
+      <c r="D33">
+        <v>6.1856229653425601</v>
+      </c>
+      <c r="E33" s="179">
+        <v>5.3914955337115598E-8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34">
+        <v>-2.3912958275121202E-2</v>
+      </c>
+      <c r="C34">
+        <v>2.82383582124828E-2</v>
+      </c>
+      <c r="D34">
+        <v>-0.84682537473267405</v>
+      </c>
+      <c r="E34">
+        <v>0.40034939026264199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35">
+        <v>1.1075393518199601E-2</v>
+      </c>
+      <c r="C35">
+        <v>2.9048737165851799E-2</v>
+      </c>
+      <c r="D35">
+        <v>0.38126936310399101</v>
+      </c>
+      <c r="E35">
+        <v>0.70430684245473196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36">
+        <v>-4.9276895852942801E-2</v>
+      </c>
+      <c r="C36">
+        <v>2.8466019978684601E-2</v>
+      </c>
+      <c r="D36">
+        <v>-1.7310778215514999</v>
+      </c>
+      <c r="E36">
+        <v>8.8411959507452897E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37">
+        <v>1.48520226552733E-2</v>
+      </c>
+      <c r="C37">
+        <v>3.55196767789204E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.41813507334862599</v>
+      </c>
+      <c r="E37">
+        <v>0.67729310091406603</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38">
+        <v>-3.8843576052541899E-2</v>
+      </c>
+      <c r="C38">
+        <v>3.0560543272458499E-2</v>
+      </c>
+      <c r="D38">
+        <v>-1.2710368302761199</v>
+      </c>
+      <c r="E38">
+        <v>0.20846372158795601</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39">
+        <v>-9.4059295797303492E-3</v>
+      </c>
+      <c r="C39">
+        <v>3.2382742731086198E-2</v>
+      </c>
+      <c r="D39">
+        <v>-0.29046117735731503</v>
+      </c>
+      <c r="E39">
+        <v>0.77243279892204997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6.1076381213912699E-2</v>
+      </c>
+      <c r="B3">
+        <v>6.81570254910878E-3</v>
+      </c>
+      <c r="C3">
+        <v>3.9489916747234198E-2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1.38806426942837E-2</v>
+      </c>
+      <c r="I3" s="179">
+        <v>3.1061025619475699E-12</v>
+      </c>
+      <c r="J3">
+        <v>3.3144078528067097E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.27539999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="179"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6">
+        <v>53.713237564633999</v>
+      </c>
+      <c r="C6">
+        <v>3.7881162415483698</v>
+      </c>
+      <c r="D6">
+        <v>14.1794058417487</v>
+      </c>
+      <c r="E6" s="179">
+        <v>1.04037532975528E-21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6">
+        <v>0.46085531896958898</v>
+      </c>
+      <c r="J6">
+        <v>2.3261536212087399E-2</v>
+      </c>
+      <c r="K6">
+        <v>19.811903855692702</v>
+      </c>
+      <c r="L6" s="179">
+        <v>1.7522479931949099E-29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7">
+        <v>8.7318604745816497</v>
+      </c>
+      <c r="C7">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D7">
+        <v>1.7180952524684101</v>
+      </c>
+      <c r="E7">
+        <v>9.0467702926530794E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7">
+        <v>2.0578482236366501E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.65938444097509197</v>
+      </c>
+      <c r="L7">
+        <v>0.51194319301494495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>4.0383975364427496</v>
+      </c>
+      <c r="C8">
+        <v>7.8855927820566798</v>
+      </c>
+      <c r="D8">
+        <v>0.51212352045770704</v>
+      </c>
+      <c r="E8">
+        <v>0.61027406389588801</v>
+      </c>
+      <c r="H8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8">
+        <v>2.9519099825737198E-3</v>
+      </c>
+      <c r="J8">
+        <v>4.8422749028052603E-2</v>
+      </c>
+      <c r="K8">
+        <v>6.0961222603524698E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.95157431831941297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9">
+        <v>-5.7687760261724899</v>
+      </c>
+      <c r="C9">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D9">
+        <v>-1.13507387480277</v>
+      </c>
+      <c r="E9">
+        <v>0.26044980027197701</v>
+      </c>
+      <c r="H9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9">
+        <v>8.1742163352924904E-2</v>
+      </c>
+      <c r="J9">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K9">
+        <v>2.6192170086922801</v>
+      </c>
+      <c r="L9">
+        <v>1.09227982377413E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>6.5340266375720297</v>
+      </c>
+      <c r="C10">
+        <v>4.8904370390048904</v>
+      </c>
+      <c r="D10">
+        <v>1.33608235531064</v>
+      </c>
+      <c r="E10">
+        <v>0.18611096316811199</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10">
+        <v>2.6801241819794999E-2</v>
+      </c>
+      <c r="J10">
+        <v>3.0030514118871698E-2</v>
+      </c>
+      <c r="K10">
+        <v>0.89246696589028995</v>
+      </c>
+      <c r="L10">
+        <v>0.37538516802156602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>3.5323492828638101</v>
+      </c>
+      <c r="C11">
+        <v>4.6394759390715503</v>
+      </c>
+      <c r="D11">
+        <v>0.76136816512312999</v>
+      </c>
+      <c r="E11">
+        <v>0.44914915404691902</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11">
+        <v>1.22967068285169E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.8489447176443802E-2</v>
+      </c>
+      <c r="K11">
+        <v>0.43162321656716102</v>
+      </c>
+      <c r="L11">
+        <v>0.66742199647298095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>-6.9176240307994004</v>
+      </c>
+      <c r="C12">
+        <v>4.2258205802240303</v>
+      </c>
+      <c r="D12">
+        <v>-1.6369895265247301</v>
+      </c>
+      <c r="E12">
+        <v>0.106392545994445</v>
+      </c>
+      <c r="H12" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12">
+        <v>-1.89314347652747E-3</v>
+      </c>
+      <c r="J12">
+        <v>2.5949330005904499E-2</v>
+      </c>
+      <c r="K12">
+        <v>-7.2955389449234298E-2</v>
+      </c>
+      <c r="L12">
+        <v>0.942062265640912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13">
+        <v>2.6418161683277899</v>
+      </c>
+      <c r="C13">
+        <v>5.7864431393956703</v>
+      </c>
+      <c r="D13">
+        <v>0.45655268784058201</v>
+      </c>
+      <c r="E13">
+        <v>0.64949157240539501</v>
+      </c>
+      <c r="H13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13">
+        <v>8.7803779901492601E-3</v>
+      </c>
+      <c r="J13">
+        <v>3.5532583490948899E-2</v>
+      </c>
+      <c r="K13">
+        <v>0.24710778467278799</v>
+      </c>
+      <c r="L13">
+        <v>0.80559186620130796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>-10.0728476070376</v>
+      </c>
+      <c r="C14">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D14">
+        <v>-1.98195008988827</v>
+      </c>
+      <c r="E14">
+        <v>5.1651703417117202E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14">
+        <v>3.0934248967801899E-4</v>
+      </c>
+      <c r="J14">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K14">
+        <v>9.91208303330148E-3</v>
+      </c>
+      <c r="L14">
+        <v>0.99212133233197997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15">
+        <v>-8.6500413492625192</v>
+      </c>
+      <c r="C15">
+        <v>7.5128319334743097</v>
+      </c>
+      <c r="D15">
+        <v>-1.15136894128048</v>
+      </c>
+      <c r="E15">
+        <v>0.25373448308222801</v>
+      </c>
+      <c r="H15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15">
+        <v>-4.3075505327091597E-2</v>
+      </c>
+      <c r="J15">
+        <v>4.6133751166095999E-2</v>
+      </c>
+      <c r="K15">
+        <v>-0.93370914435304098</v>
+      </c>
+      <c r="L15">
+        <v>0.35385743446773898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16">
+        <v>-3.93800857656541</v>
+      </c>
+      <c r="C16">
+        <v>7.7014679504967001</v>
+      </c>
+      <c r="D16">
+        <v>-0.51133220340304497</v>
+      </c>
+      <c r="E16">
+        <v>0.61082491583855203</v>
+      </c>
+      <c r="H16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16">
+        <v>-1.5983525492887701E-2</v>
+      </c>
+      <c r="J16">
+        <v>4.7292100926523799E-2</v>
+      </c>
+      <c r="K16">
+        <v>-0.33797452808706502</v>
+      </c>
+      <c r="L16">
+        <v>0.736455073633836</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17">
+        <v>-2.7170521218343602</v>
+      </c>
+      <c r="C17">
+        <v>6.4632757955015201</v>
+      </c>
+      <c r="D17">
+        <v>-0.42038313199096999</v>
+      </c>
+      <c r="E17">
+        <v>0.67557115913499199</v>
+      </c>
+      <c r="H17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I17">
+        <v>-2.93493724345451E-2</v>
+      </c>
+      <c r="J17">
+        <v>3.9688783125703099E-2</v>
+      </c>
+      <c r="K17">
+        <v>-0.73948783820328401</v>
+      </c>
+      <c r="L17">
+        <v>0.462232965617632</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18">
+        <v>0.37646142367103103</v>
+      </c>
+      <c r="C18">
+        <v>6.6696668915618202</v>
+      </c>
+      <c r="D18">
+        <v>5.6443811931194597E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.95515878597181803</v>
+      </c>
+      <c r="H18" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18">
+        <v>-2.67907261490406E-4</v>
+      </c>
+      <c r="J18">
+        <v>4.09561608007072E-2</v>
+      </c>
+      <c r="K18">
+        <v>-6.5413177468963404E-3</v>
+      </c>
+      <c r="L18">
+        <v>0.99480055281438395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19">
+        <v>18.609694944960701</v>
+      </c>
+      <c r="C19">
+        <v>6.9620771936116697</v>
+      </c>
+      <c r="D19">
+        <v>2.6730089924938998</v>
+      </c>
+      <c r="E19">
+        <v>9.4629519978275903E-3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19">
+        <v>8.5207167240391804E-2</v>
+      </c>
+      <c r="J19">
+        <v>4.2751753226123297E-2</v>
+      </c>
+      <c r="K19">
+        <v>1.9930683728855001</v>
+      </c>
+      <c r="L19">
+        <v>5.0390944266193803E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20">
+        <v>21.876220481084701</v>
+      </c>
+      <c r="C20">
+        <v>7.2912744934245799</v>
+      </c>
+      <c r="D20">
+        <v>3.0003287492211599</v>
+      </c>
+      <c r="E20">
+        <v>3.8026406271824799E-3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20">
+        <v>0.120858551679667</v>
+      </c>
+      <c r="J20">
+        <v>4.4773242119872103E-2</v>
+      </c>
+      <c r="K20">
+        <v>2.6993477791063301</v>
+      </c>
+      <c r="L20">
+        <v>8.81511325827764E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25">
+        <v>53.713237564633999</v>
+      </c>
+      <c r="C25">
+        <v>3.7881162415483698</v>
+      </c>
+      <c r="D25">
+        <v>14.1794058417487</v>
+      </c>
+      <c r="E25" s="179">
+        <v>1.04037532975528E-21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25">
+        <v>0.46085531896958898</v>
+      </c>
+      <c r="J25">
+        <v>2.3261536212087399E-2</v>
+      </c>
+      <c r="K25">
+        <v>19.811903855692702</v>
+      </c>
+      <c r="L25" s="179">
+        <v>1.75224799319486E-29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26">
+        <v>-5.7687760261724899</v>
+      </c>
+      <c r="C26">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D26">
+        <v>-1.13507387480277</v>
+      </c>
+      <c r="E26">
+        <v>0.26044980027197701</v>
+      </c>
+      <c r="H26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26">
+        <v>8.1742163352924793E-2</v>
+      </c>
+      <c r="J26">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K26">
+        <v>2.6192170086922801</v>
+      </c>
+      <c r="L26">
+        <v>1.09227982377413E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27">
+        <v>6.5340266375720297</v>
+      </c>
+      <c r="C27">
+        <v>4.8904370390048904</v>
+      </c>
+      <c r="D27">
+        <v>1.33608235531064</v>
+      </c>
+      <c r="E27">
+        <v>0.18611096316811199</v>
+      </c>
+      <c r="H27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27">
+        <v>2.6801241819794999E-2</v>
+      </c>
+      <c r="J27">
+        <v>3.0030514118871698E-2</v>
+      </c>
+      <c r="K27">
+        <v>0.89246696589028995</v>
+      </c>
+      <c r="L27">
+        <v>0.37538516802156602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28">
+        <v>3.5323492828638101</v>
+      </c>
+      <c r="C28">
+        <v>4.6394759390715503</v>
+      </c>
+      <c r="D28">
+        <v>0.76136816512312899</v>
+      </c>
+      <c r="E28">
+        <v>0.44914915404691902</v>
+      </c>
+      <c r="H28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28">
+        <v>1.22967068285169E-2</v>
+      </c>
+      <c r="J28">
+        <v>2.8489447176443802E-2</v>
+      </c>
+      <c r="K28">
+        <v>0.43162321656716102</v>
+      </c>
+      <c r="L28">
+        <v>0.66742199647298095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29">
+        <v>1.81423644378225</v>
+      </c>
+      <c r="C29">
+        <v>4.5527491154401902</v>
+      </c>
+      <c r="D29">
+        <v>0.398492514693913</v>
+      </c>
+      <c r="E29">
+        <v>0.69155343838387096</v>
+      </c>
+      <c r="H29" t="s">
+        <v>125</v>
+      </c>
+      <c r="I29">
+        <v>1.8685338759839E-2</v>
+      </c>
+      <c r="J29">
+        <v>2.7956887186247802E-2</v>
+      </c>
+      <c r="K29">
+        <v>0.66836263405714402</v>
+      </c>
+      <c r="L29">
+        <v>0.506232967950767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30">
+        <v>6.6802137047705399</v>
+      </c>
+      <c r="C30">
+        <v>5.3572053646434998</v>
+      </c>
+      <c r="D30">
+        <v>1.2469586752934001</v>
+      </c>
+      <c r="E30">
+        <v>0.21681972818089901</v>
+      </c>
+      <c r="H30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30">
+        <v>1.1732287972723E-2</v>
+      </c>
+      <c r="J30">
+        <v>3.2896779992766897E-2</v>
+      </c>
+      <c r="K30">
+        <v>0.35663940286260898</v>
+      </c>
+      <c r="L30">
+        <v>0.72249945117350201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31">
+        <v>0.100388959877335</v>
+      </c>
+      <c r="C31">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D31">
+        <v>1.9752697133396901E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.98430024750457701</v>
+      </c>
+      <c r="H31" t="s">
+        <v>135</v>
+      </c>
+      <c r="I31">
+        <v>-1.3031615510313999E-2</v>
+      </c>
+      <c r="J31">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K31">
+        <v>-0.41756454191191</v>
+      </c>
+      <c r="L31">
+        <v>0.67762082405570401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32">
+        <v>-1.3409871324559</v>
+      </c>
+      <c r="C32">
+        <v>5.3572053646434998</v>
+      </c>
+      <c r="D32">
+        <v>-0.25031467737006202</v>
+      </c>
+      <c r="E32">
+        <v>0.80312156418173397</v>
+      </c>
+      <c r="H32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32">
+        <v>2.0887824726044502E-2</v>
+      </c>
+      <c r="J32">
+        <v>3.2896779992766897E-2</v>
+      </c>
+      <c r="K32">
+        <v>0.63495043377002802</v>
+      </c>
+      <c r="L32">
+        <v>0.52765588116031004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33">
+        <v>8.7318604745816604</v>
+      </c>
+      <c r="C33">
+        <v>5.0822912536639002</v>
+      </c>
+      <c r="D33">
+        <v>1.7180952524684101</v>
+      </c>
+      <c r="E33">
+        <v>9.0467702926530794E-2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33">
+        <v>2.0578482236366501E-2</v>
+      </c>
+      <c r="J33">
+        <v>3.12086257387802E-2</v>
+      </c>
+      <c r="K33">
+        <v>0.65938444097509297</v>
+      </c>
+      <c r="L33">
+        <v>0.51194319301494495</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34">
+        <v>-2.7170521218343602</v>
+      </c>
+      <c r="C34">
+        <v>6.4632757955015201</v>
+      </c>
+      <c r="D34">
+        <v>-0.42038313199096999</v>
+      </c>
+      <c r="E34">
+        <v>0.67557115913499199</v>
+      </c>
+      <c r="H34" t="s">
+        <v>130</v>
+      </c>
+      <c r="I34">
+        <v>-2.93493724345451E-2</v>
+      </c>
+      <c r="J34">
+        <v>3.9688783125703099E-2</v>
+      </c>
+      <c r="K34">
+        <v>-0.73948783820328401</v>
+      </c>
+      <c r="L34">
+        <v>0.462232965617631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35">
+        <v>0.37646142367103702</v>
+      </c>
+      <c r="C35">
+        <v>6.6696668915618202</v>
+      </c>
+      <c r="D35">
+        <v>5.6443811931195603E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.95515878597181803</v>
+      </c>
+      <c r="H35" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35">
+        <v>-2.6790726149040399E-4</v>
+      </c>
+      <c r="J35">
+        <v>4.09561608007072E-2</v>
+      </c>
+      <c r="K35">
+        <v>-6.5413177468962797E-3</v>
+      </c>
+      <c r="L35">
+        <v>0.99480055281438395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36">
+        <v>9.9596535956981604</v>
+      </c>
+      <c r="C36">
+        <v>6.6096326647790002</v>
+      </c>
+      <c r="D36">
+        <v>1.5068391998197599</v>
+      </c>
+      <c r="E36">
+        <v>0.13662358948439801</v>
+      </c>
+      <c r="H36" t="s">
+        <v>132</v>
+      </c>
+      <c r="I36">
+        <v>4.2131661913300297E-2</v>
+      </c>
+      <c r="J36">
+        <v>4.0587510988709198E-2</v>
+      </c>
+      <c r="K36">
+        <v>1.03804497706254</v>
+      </c>
+      <c r="L36">
+        <v>0.30303725437492501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37">
+        <v>-3.9380085765653998</v>
+      </c>
+      <c r="C37">
+        <v>7.7014679504967001</v>
+      </c>
+      <c r="D37">
+        <v>-0.51133220340304397</v>
+      </c>
+      <c r="E37">
+        <v>0.61082491583855303</v>
+      </c>
+      <c r="H37" t="s">
+        <v>133</v>
+      </c>
+      <c r="I37">
+        <v>-1.5983525492887701E-2</v>
+      </c>
+      <c r="J37">
+        <v>4.7292100926523799E-2</v>
+      </c>
+      <c r="K37">
+        <v>-0.33797452808706502</v>
+      </c>
+      <c r="L37">
+        <v>0.736455073633836</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38">
+        <v>13.2261791318222</v>
+      </c>
+      <c r="C38">
+        <v>6.95553081022359</v>
+      </c>
+      <c r="D38">
+        <v>1.9015341161858801</v>
+      </c>
+      <c r="E38">
+        <v>6.1598607502696003E-2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>134</v>
+      </c>
+      <c r="I38">
+        <v>7.7783046352575297E-2</v>
+      </c>
+      <c r="J38">
+        <v>4.2711554107476998E-2</v>
+      </c>
+      <c r="K38">
+        <v>1.82112423623936</v>
+      </c>
+      <c r="L38">
+        <v>7.3120780208466796E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39">
+        <v>-8.6500413492625299</v>
+      </c>
+      <c r="C39">
+        <v>7.5128319334743097</v>
+      </c>
+      <c r="D39">
+        <v>-1.15136894128048</v>
+      </c>
+      <c r="E39">
+        <v>0.25373448308222801</v>
+      </c>
+      <c r="H39" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39">
+        <v>-4.3075505327091701E-2</v>
+      </c>
+      <c r="J39">
+        <v>4.6133751166095999E-2</v>
+      </c>
+      <c r="K39">
+        <v>-0.93370914435304297</v>
+      </c>
+      <c r="L39">
+        <v>0.35385743446773799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
@@ -3540,7 +6609,7 @@
       <c r="D2">
         <v>55.202091892640198</v>
       </c>
-      <c r="E2" s="179">
+      <c r="E2" s="180">
         <v>1.19324726915733E-87</v>
       </c>
     </row>
@@ -3608,7 +6677,7 @@
       <c r="D6">
         <v>4.9737234773683001</v>
       </c>
-      <c r="E6" s="179">
+      <c r="E6" s="180">
         <v>2.1942601887269799E-6</v>
       </c>
     </row>
@@ -3761,7 +6830,7 @@
       <c r="D15">
         <v>4.1874552442768103</v>
       </c>
-      <c r="E15" s="179">
+      <c r="E15" s="180">
         <v>5.3828401638443797E-5</v>
       </c>
     </row>
@@ -3849,7 +6918,7 @@
       <c r="D2">
         <v>55.202091892640297</v>
       </c>
-      <c r="E2" s="179">
+      <c r="E2" s="180">
         <v>1.1932472691573001E-87</v>
       </c>
     </row>
@@ -3883,7 +6952,7 @@
       <c r="D4">
         <v>4.9737234773683001</v>
       </c>
-      <c r="E4" s="179">
+      <c r="E4" s="180">
         <v>2.1942601887269799E-6</v>
       </c>
     </row>
@@ -3934,7 +7003,7 @@
       <c r="D7">
         <v>4.70271882771873</v>
       </c>
-      <c r="E7" s="179">
+      <c r="E7" s="180">
         <v>6.8714024562480201E-6</v>
       </c>
     </row>
@@ -4154,7 +7223,7 @@
       <c r="D2">
         <v>52.600360368144997</v>
       </c>
-      <c r="E2" s="179">
+      <c r="E2" s="180">
         <v>3.2469395311454599E-56</v>
       </c>
     </row>
@@ -4205,7 +7274,7 @@
       <c r="D5">
         <v>4.7393067601475396</v>
       </c>
-      <c r="E5" s="179">
+      <c r="E5" s="180">
         <v>1.15885934666249E-5</v>
       </c>
     </row>
@@ -4304,7 +7373,7 @@
       <c r="D12">
         <v>52.600360368144997</v>
       </c>
-      <c r="E12" s="179">
+      <c r="E12" s="180">
         <v>3.2469395311454599E-56</v>
       </c>
     </row>
@@ -4321,7 +7390,7 @@
       <c r="D13">
         <v>4.7393067601475503</v>
       </c>
-      <c r="E13" s="179">
+      <c r="E13" s="180">
         <v>1.15885934666249E-5</v>
       </c>
     </row>
@@ -4372,7 +7441,7 @@
       <c r="D16">
         <v>4.4810748391411099</v>
       </c>
-      <c r="E16" s="179">
+      <c r="E16" s="180">
         <v>2.9724948876506599E-5</v>
       </c>
     </row>
@@ -4436,8 +7505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4476,7 +7545,7 @@
       <c r="D2">
         <v>47.938226170892698</v>
       </c>
-      <c r="E2" s="179">
+      <c r="E2" s="180">
         <v>3.70900312056121E-47</v>
       </c>
     </row>
@@ -4578,7 +7647,7 @@
       <c r="D8">
         <v>5.8108292810398297</v>
       </c>
-      <c r="E8" s="179">
+      <c r="E8" s="180">
         <v>3.0812815812629402E-7</v>
       </c>
     </row>
@@ -4595,7 +7664,7 @@
       <c r="D9">
         <v>6.9952918777234796</v>
       </c>
-      <c r="E9" s="179">
+      <c r="E9" s="180">
         <v>3.5233981084583199E-9</v>
       </c>
     </row>
@@ -4694,7 +7763,7 @@
       <c r="D16">
         <v>47.938226170892698</v>
       </c>
-      <c r="E16" s="179">
+      <c r="E16" s="180">
         <v>3.70900312056121E-47</v>
       </c>
     </row>
@@ -4762,7 +7831,7 @@
       <c r="D20">
         <v>6.4462171616031299</v>
       </c>
-      <c r="E20" s="179">
+      <c r="E20" s="180">
         <v>2.83192416946778E-8</v>
       </c>
     </row>
@@ -4779,7 +7848,7 @@
       <c r="D21">
         <v>7.2896050726363102</v>
       </c>
-      <c r="E21" s="179">
+      <c r="E21" s="180">
         <v>1.1495244749831801E-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates DOIs to ref. Moved Tables around
</commit_message>
<xml_diff>
--- a/doc/MainTables.xlsx
+++ b/doc/MainTables.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8910" windowHeight="6435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8910" windowHeight="6435" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1 Strain.Info" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 1 MLH1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2 Models" sheetId="4" r:id="rId2"/>
-    <sheet name="Table 3 MLH1" sheetId="1" r:id="rId3"/>
-    <sheet name="Table 4 DMC1" sheetId="2" r:id="rId4"/>
+    <sheet name="Table 3 DMC1" sheetId="2" r:id="rId3"/>
+    <sheet name="Table 4 Strain.Info" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>sex*strain</t>
-  </si>
-  <si>
-    <t>Model</t>
   </si>
   <si>
     <t>PWD/PhJ</t>
@@ -477,6 +474,9 @@
   </si>
   <si>
     <t>males from 12 strains</t>
+  </si>
+  <si>
+    <t>Model    APRIL REMOVE the equations below</t>
   </si>
 </sst>
 </file>
@@ -1310,64 +1310,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1431,8 +1431,8 @@
       <xdr:rowOff>106913</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2514600" cy="509820"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1497,7 +1497,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1509,7 +1509,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1521,7 +1521,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1533,7 +1533,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1545,7 +1545,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1557,7 +1557,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1569,7 +1569,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1581,7 +1581,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1593,7 +1593,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1605,7 +1605,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1617,7 +1617,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1629,7 +1629,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1641,7 +1641,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1653,7 +1653,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1665,7 +1665,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1677,7 +1677,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1689,7 +1689,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1714,7 +1714,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1806,8 +1806,8 @@
       <xdr:rowOff>184669</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2514600" cy="509820"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1872,7 +1872,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1884,7 +1884,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1896,7 +1896,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1908,7 +1908,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1920,7 +1920,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1932,7 +1932,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1944,7 +1944,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1956,7 +1956,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1968,7 +1968,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1980,7 +1980,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1992,7 +1992,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2004,7 +2004,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2016,7 +2016,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2028,7 +2028,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2040,7 +2040,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2065,7 +2065,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2157,8 +2157,8 @@
       <xdr:rowOff>87475</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2514600" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -2223,7 +2223,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2235,7 +2235,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2247,7 +2247,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2259,7 +2259,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2271,7 +2271,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2283,7 +2283,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2295,7 +2295,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2307,7 +2307,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2319,7 +2319,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2331,7 +2331,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2343,7 +2343,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2355,7 +2355,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2367,7 +2367,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2389,7 +2389,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -2478,8 +2478,8 @@
       <xdr:rowOff>220437</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2802294" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -2544,7 +2544,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2556,7 +2556,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2568,7 +2568,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2580,7 +2580,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2592,7 +2592,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2604,7 +2604,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2616,7 +2616,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2628,7 +2628,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2640,7 +2640,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2652,7 +2652,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2664,7 +2664,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2676,7 +2676,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2688,7 +2688,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2700,7 +2700,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2712,7 +2712,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2724,7 +2724,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2736,7 +2736,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2758,7 +2758,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -2847,8 +2847,8 @@
       <xdr:rowOff>120133</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2873440" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -2913,7 +2913,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2925,7 +2925,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2937,7 +2937,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2949,7 +2949,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2961,7 +2961,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2973,7 +2973,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2985,7 +2985,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2997,7 +2997,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3009,7 +3009,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3021,7 +3021,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3033,7 +3033,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3045,7 +3045,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3057,7 +3057,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3069,7 +3069,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3081,7 +3081,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3093,7 +3093,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3105,7 +3105,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3127,7 +3127,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -3216,8 +3216,8 @@
       <xdr:rowOff>136462</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2808515" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -3282,7 +3282,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3294,7 +3294,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3306,7 +3306,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3318,7 +3318,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3330,7 +3330,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3342,7 +3342,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3354,7 +3354,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3366,7 +3366,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3378,7 +3378,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3390,7 +3390,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3402,7 +3402,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3414,7 +3414,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3426,7 +3426,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3438,7 +3438,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3450,7 +3450,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3472,7 +3472,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -3561,8 +3561,8 @@
       <xdr:rowOff>181949</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2860223" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -3627,7 +3627,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3639,7 +3639,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3651,7 +3651,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3663,7 +3663,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3675,7 +3675,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3687,7 +3687,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3699,7 +3699,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3711,7 +3711,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3723,7 +3723,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3735,7 +3735,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3747,7 +3747,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3759,7 +3759,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3771,7 +3771,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3783,7 +3783,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3795,7 +3795,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -3817,7 +3817,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -4164,10 +4164,1373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U29"/>
+  <sheetViews>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="13" max="14" width="4.5703125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="147" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="160" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="36">
+        <v>14</v>
+      </c>
+      <c r="F2" s="37">
+        <v>184</v>
+      </c>
+      <c r="G2" s="38">
+        <v>24.701000000000001</v>
+      </c>
+      <c r="H2" s="39">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I2" s="39">
+        <v>14.638271224837814</v>
+      </c>
+      <c r="J2" s="40">
+        <v>13.074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="148"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="41">
+        <v>11</v>
+      </c>
+      <c r="F3" s="42">
+        <v>222</v>
+      </c>
+      <c r="G3" s="43">
+        <v>23.382999999999999</v>
+      </c>
+      <c r="H3" s="44">
+        <v>0.18</v>
+      </c>
+      <c r="I3" s="44">
+        <v>11.479933887268658</v>
+      </c>
+      <c r="J3" s="45">
+        <v>7.2060000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="148"/>
+      <c r="B4" s="153"/>
+      <c r="C4" s="160" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="41">
+        <v>12</v>
+      </c>
+      <c r="F4" s="42">
+        <v>318</v>
+      </c>
+      <c r="G4" s="43">
+        <v>28.210999999999999</v>
+      </c>
+      <c r="H4" s="44">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="I4" s="44">
+        <v>14.835969061582837</v>
+      </c>
+      <c r="J4" s="45">
+        <v>17.516999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="148"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="41">
+        <v>18</v>
+      </c>
+      <c r="F5" s="42">
+        <v>355</v>
+      </c>
+      <c r="G5" s="43">
+        <v>23.161000000000001</v>
+      </c>
+      <c r="H5" s="44">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I5" s="44">
+        <v>11.35380583435758</v>
+      </c>
+      <c r="J5" s="45">
+        <v>6.915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="148"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="41">
+        <v>9</v>
+      </c>
+      <c r="F6" s="42">
+        <v>147</v>
+      </c>
+      <c r="G6" s="43">
+        <v>26.585000000000001</v>
+      </c>
+      <c r="H6" s="44">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="I6" s="44">
+        <v>18.16189516714001</v>
+      </c>
+      <c r="J6" s="45">
+        <v>23.312999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="148"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="41">
+        <v>10</v>
+      </c>
+      <c r="F7" s="42">
+        <v>253</v>
+      </c>
+      <c r="G7" s="43">
+        <v>24.161999999999999</v>
+      </c>
+      <c r="H7" s="44">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I7" s="44">
+        <v>12.83701437670674</v>
+      </c>
+      <c r="J7" s="45">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="148"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="46">
+        <v>1</v>
+      </c>
+      <c r="F8" s="47">
+        <v>26</v>
+      </c>
+      <c r="G8" s="48">
+        <v>21.808</v>
+      </c>
+      <c r="H8" s="46">
+        <v>0.41</v>
+      </c>
+      <c r="I8" s="46">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="J8" s="49">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="148"/>
+      <c r="B9" s="152" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="41">
+        <v>15</v>
+      </c>
+      <c r="F9" s="42">
+        <v>222</v>
+      </c>
+      <c r="G9" s="43">
+        <v>25.977</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0.251</v>
+      </c>
+      <c r="I9" s="43">
+        <v>14.41018621027294</v>
+      </c>
+      <c r="J9" s="45">
+        <v>14.013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="148"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="41">
+        <v>8</v>
+      </c>
+      <c r="F10" s="42">
+        <v>161</v>
+      </c>
+      <c r="G10" s="43">
+        <v>28.670999999999999</v>
+      </c>
+      <c r="H10" s="45">
+        <v>0.246</v>
+      </c>
+      <c r="I10" s="43">
+        <v>10.896284161204306</v>
+      </c>
+      <c r="J10" s="45">
+        <v>9.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="148"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="160" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="41">
+        <v>1</v>
+      </c>
+      <c r="F11" s="42">
+        <v>32</v>
+      </c>
+      <c r="G11" s="43">
+        <v>25.937999999999999</v>
+      </c>
+      <c r="H11" s="45">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="I11" s="43">
+        <v>12.070868672504577</v>
+      </c>
+      <c r="J11" s="45">
+        <v>9.8019999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="148"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="161"/>
+      <c r="D12" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="41">
+        <v>3</v>
+      </c>
+      <c r="F12" s="42">
+        <v>86</v>
+      </c>
+      <c r="G12" s="43">
+        <v>26.081</v>
+      </c>
+      <c r="H12" s="45">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="I12" s="43">
+        <v>10.408689886052935</v>
+      </c>
+      <c r="J12" s="45">
+        <v>7.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="148"/>
+      <c r="B13" s="153"/>
+      <c r="C13" s="160" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="41">
+        <v>9</v>
+      </c>
+      <c r="F13" s="42">
+        <v>184</v>
+      </c>
+      <c r="G13" s="43">
+        <v>25.625</v>
+      </c>
+      <c r="H13" s="45">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="I13" s="43">
+        <v>15.628736960600049</v>
+      </c>
+      <c r="J13" s="45">
+        <v>16.039000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="148"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="41">
+        <v>13</v>
+      </c>
+      <c r="F14" s="42">
+        <v>264</v>
+      </c>
+      <c r="G14" s="43">
+        <v>22.989000000000001</v>
+      </c>
+      <c r="H14" s="45">
+        <v>0.186</v>
+      </c>
+      <c r="I14" s="43">
+        <v>13.159636243359548</v>
+      </c>
+      <c r="J14" s="45">
+        <v>9.1519999999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="148"/>
+      <c r="B15" s="153"/>
+      <c r="C15" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="41">
+        <v>3</v>
+      </c>
+      <c r="F15" s="42">
+        <v>62</v>
+      </c>
+      <c r="G15" s="43">
+        <v>22.3</v>
+      </c>
+      <c r="H15" s="50">
+        <v>0.32</v>
+      </c>
+      <c r="I15" s="42">
+        <v>11.21</v>
+      </c>
+      <c r="J15" s="50">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="148"/>
+      <c r="B16" s="153"/>
+      <c r="C16" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="41">
+        <v>3</v>
+      </c>
+      <c r="F16" s="42">
+        <v>63</v>
+      </c>
+      <c r="G16" s="42">
+        <v>24.41</v>
+      </c>
+      <c r="H16" s="50">
+        <v>0.33</v>
+      </c>
+      <c r="I16" s="42">
+        <v>10.65</v>
+      </c>
+      <c r="J16" s="50">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="148"/>
+      <c r="B17" s="154"/>
+      <c r="C17" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="46">
+        <v>2</v>
+      </c>
+      <c r="F17" s="47">
+        <v>10</v>
+      </c>
+      <c r="G17" s="48">
+        <v>23.7</v>
+      </c>
+      <c r="H17" s="49">
+        <v>1.18</v>
+      </c>
+      <c r="I17" s="47">
+        <v>15.79</v>
+      </c>
+      <c r="J17" s="49">
+        <v>14.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="148"/>
+      <c r="B18" s="152" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="150" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="51">
+        <v>1</v>
+      </c>
+      <c r="F18" s="52">
+        <v>1</v>
+      </c>
+      <c r="G18" s="53">
+        <v>26</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="148"/>
+      <c r="B19" s="153"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="51">
+        <v>2</v>
+      </c>
+      <c r="F19" s="52">
+        <v>44</v>
+      </c>
+      <c r="G19" s="53">
+        <v>22</v>
+      </c>
+      <c r="H19" s="55">
+        <v>0.34</v>
+      </c>
+      <c r="I19" s="55">
+        <v>10</v>
+      </c>
+      <c r="J19" s="55">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="148"/>
+      <c r="B20" s="154"/>
+      <c r="C20" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="56">
+        <v>4</v>
+      </c>
+      <c r="F20" s="57">
+        <v>44</v>
+      </c>
+      <c r="G20" s="58">
+        <v>24</v>
+      </c>
+      <c r="H20" s="59">
+        <v>0.41</v>
+      </c>
+      <c r="I20" s="59">
+        <v>11</v>
+      </c>
+      <c r="J20" s="59">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="148"/>
+      <c r="B21" s="155" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="60">
+        <v>14</v>
+      </c>
+      <c r="F21" s="60">
+        <v>300</v>
+      </c>
+      <c r="G21" s="61">
+        <v>28.123000000000001</v>
+      </c>
+      <c r="H21" s="62">
+        <v>0.254</v>
+      </c>
+      <c r="I21" s="62">
+        <v>15.64239374084605</v>
+      </c>
+      <c r="J21" s="63">
+        <v>19.353000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="148"/>
+      <c r="B22" s="155"/>
+      <c r="C22" s="159"/>
+      <c r="D22" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="42">
+        <v>7</v>
+      </c>
+      <c r="F22" s="42">
+        <v>166</v>
+      </c>
+      <c r="G22" s="43">
+        <v>30.367000000000001</v>
+      </c>
+      <c r="H22" s="44">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="I22" s="44">
+        <v>10.262658213499735</v>
+      </c>
+      <c r="J22" s="45">
+        <v>9.7129999999999992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="148"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="156" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="42">
+        <v>1</v>
+      </c>
+      <c r="F23" s="42">
+        <v>21</v>
+      </c>
+      <c r="G23" s="43">
+        <v>27.619</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="I23" s="44">
+        <v>15.338917885642941</v>
+      </c>
+      <c r="J23" s="45">
+        <v>17.948</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="149"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="64">
+        <v>6</v>
+      </c>
+      <c r="F24" s="64">
+        <v>119</v>
+      </c>
+      <c r="G24" s="65">
+        <v>23.42</v>
+      </c>
+      <c r="H24" s="66">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="I24" s="66">
+        <v>10.80040516644884</v>
+      </c>
+      <c r="J24" s="67">
+        <v>6.3979999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="163" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="147"/>
+      <c r="C25" s="156" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="42">
+        <v>2</v>
+      </c>
+      <c r="F25" s="42">
+        <v>2</v>
+      </c>
+      <c r="G25" s="43">
+        <v>26</v>
+      </c>
+      <c r="H25" s="45">
+        <v>2</v>
+      </c>
+      <c r="I25" s="45">
+        <v>10.878565864408424</v>
+      </c>
+      <c r="J25" s="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="164"/>
+      <c r="B26" s="149"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="42">
+        <v>5</v>
+      </c>
+      <c r="F26" s="42">
+        <v>103</v>
+      </c>
+      <c r="G26" s="43">
+        <v>24.427</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0.246</v>
+      </c>
+      <c r="I26" s="45">
+        <v>10.232121984584271</v>
+      </c>
+      <c r="J26" s="68">
+        <v>6.2469999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="163" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="147"/>
+      <c r="C27" s="156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="37">
+        <v>6</v>
+      </c>
+      <c r="F27" s="37">
+        <v>97</v>
+      </c>
+      <c r="G27" s="38">
+        <v>28.236999999999998</v>
+      </c>
+      <c r="H27" s="40">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="I27" s="40">
+        <v>15.628316890383017</v>
+      </c>
+      <c r="J27" s="69">
+        <v>19.474</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="164"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="64">
+        <v>4</v>
+      </c>
+      <c r="F28" s="64">
+        <v>133</v>
+      </c>
+      <c r="G28" s="65">
+        <v>25.774000000000001</v>
+      </c>
+      <c r="H28" s="67">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="I28" s="67">
+        <v>10.781039022222362</v>
+      </c>
+      <c r="J28" s="70">
+        <v>7.7210000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="145" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="146"/>
+      <c r="C29" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="71">
+        <v>2</v>
+      </c>
+      <c r="F29" s="72">
+        <v>57</v>
+      </c>
+      <c r="G29" s="73">
+        <v>27</v>
+      </c>
+      <c r="H29" s="74">
+        <v>0.4</v>
+      </c>
+      <c r="I29" s="74">
+        <v>11</v>
+      </c>
+      <c r="J29" s="75">
+        <v>8.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A2:A24"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C27:C28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="104" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="104" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="136" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="139" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="137"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="138"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="136" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="142" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="137"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="137"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="137"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="137"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="138"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="142" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="137"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="138"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="136" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="137"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="138"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="136" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="137"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="138"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="136" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="138"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="136" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="138"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="174" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="165" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="166"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="168" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="169"/>
+      <c r="H1" s="170"/>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="175"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="92" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="33">
+        <v>21</v>
+      </c>
+      <c r="D3" s="94">
+        <v>177.76190476190476</v>
+      </c>
+      <c r="E3" s="95">
+        <v>0.13715946228965248</v>
+      </c>
+      <c r="F3" s="96">
+        <v>20</v>
+      </c>
+      <c r="G3" s="94">
+        <v>144.25</v>
+      </c>
+      <c r="H3" s="95">
+        <v>0.16902410587679217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="171"/>
+      <c r="B4" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="33">
+        <v>19</v>
+      </c>
+      <c r="D4" s="94">
+        <v>158.15789473684211</v>
+      </c>
+      <c r="E4" s="95">
+        <v>0.15299197633573675</v>
+      </c>
+      <c r="F4" s="96">
+        <v>9</v>
+      </c>
+      <c r="G4" s="94">
+        <v>131.77777777777777</v>
+      </c>
+      <c r="H4" s="95">
+        <v>0.18361888701517706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="171"/>
+      <c r="B5" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="33">
+        <v>1</v>
+      </c>
+      <c r="D5" s="94">
+        <v>159</v>
+      </c>
+      <c r="E5" s="95">
+        <v>0.15241074020319303</v>
+      </c>
+      <c r="F5" s="96">
+        <v>11</v>
+      </c>
+      <c r="G5" s="94">
+        <v>167.36363636363637</v>
+      </c>
+      <c r="H5" s="95">
+        <v>0.1447943425395897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="172" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="32">
+        <v>18</v>
+      </c>
+      <c r="D6" s="97">
+        <v>180.22222222222223</v>
+      </c>
+      <c r="E6" s="98">
+        <v>0.16261243834771885</v>
+      </c>
+      <c r="F6" s="99">
+        <v>18</v>
+      </c>
+      <c r="G6" s="97">
+        <v>140.77777777777777</v>
+      </c>
+      <c r="H6" s="98">
+        <v>0.20817472375690607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="173"/>
+      <c r="B7" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="34">
+        <v>17</v>
+      </c>
+      <c r="D7" s="100">
+        <v>231</v>
+      </c>
+      <c r="E7" s="101">
+        <v>0.13518614718614719</v>
+      </c>
+      <c r="F7" s="102">
+        <v>17</v>
+      </c>
+      <c r="G7" s="100">
+        <v>164.41176470588235</v>
+      </c>
+      <c r="H7" s="101">
+        <v>0.1899377459749553</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,13 +5547,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="106" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" s="105" t="s">
         <v>42</v>
@@ -4205,31 +5568,31 @@
         <v>10</v>
       </c>
       <c r="D2" s="108" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="131"/>
       <c r="B3" s="110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="111" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="131"/>
       <c r="B4" s="110" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="111" t="s">
         <v>38</v>
@@ -4238,22 +5601,22 @@
         <v>39</v>
       </c>
       <c r="E4" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="132"/>
       <c r="B5" s="113" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="114" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="114" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4261,91 +5624,91 @@
         <v>12</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="108" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="109" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="134"/>
       <c r="B7" s="117" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="111" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="111" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="134"/>
       <c r="B8" s="118" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="111" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="111" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="112" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="134"/>
       <c r="B9" s="118" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="111" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="134"/>
       <c r="B10" s="117" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="111" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="111" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="135"/>
       <c r="B11" s="120" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="114" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="114" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4353,31 +5716,31 @@
         <v>16</v>
       </c>
       <c r="B12" s="113" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="108" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="121" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="132"/>
       <c r="B13" s="113" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="114" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4385,7 +5748,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="122" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="108" t="s">
         <v>35</v>
@@ -4394,22 +5757,22 @@
         <v>37</v>
       </c>
       <c r="E14" s="109" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="132"/>
       <c r="B15" s="123" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="114" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="123" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="115" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4417,16 +5780,16 @@
         <v>19</v>
       </c>
       <c r="B16" s="124" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="108" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="125" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4434,16 +5797,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="108" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="125" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="109" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4451,7 +5814,7 @@
         <v>45</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="126" t="s">
         <v>43</v>
@@ -4460,7 +5823,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="127" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4496,1367 +5859,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="104" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="104" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="104" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="139" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="137"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="138"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="136" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="142" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="137"/>
-      <c r="B6" s="143"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="137"/>
-      <c r="B7" s="143"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="143"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="143"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="138"/>
-      <c r="B10" s="144"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="136" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="142" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="143"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="138"/>
-      <c r="B13" s="144"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="136" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="136" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="136" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="136" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="138"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
-  <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="13" max="14" width="4.5703125" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="158" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="145" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="36">
-        <v>14</v>
-      </c>
-      <c r="F2" s="37">
-        <v>184</v>
-      </c>
-      <c r="G2" s="38">
-        <v>24.701000000000001</v>
-      </c>
-      <c r="H2" s="39">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="I2" s="39">
-        <v>14.638271224837814</v>
-      </c>
-      <c r="J2" s="40">
-        <v>13.074</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="155"/>
-      <c r="B3" s="159"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="41">
-        <v>11</v>
-      </c>
-      <c r="F3" s="42">
-        <v>222</v>
-      </c>
-      <c r="G3" s="43">
-        <v>23.382999999999999</v>
-      </c>
-      <c r="H3" s="44">
-        <v>0.18</v>
-      </c>
-      <c r="I3" s="44">
-        <v>11.479933887268658</v>
-      </c>
-      <c r="J3" s="45">
-        <v>7.2060000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="155"/>
-      <c r="B4" s="159"/>
-      <c r="C4" s="145" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="41">
-        <v>12</v>
-      </c>
-      <c r="F4" s="42">
-        <v>318</v>
-      </c>
-      <c r="G4" s="43">
-        <v>28.210999999999999</v>
-      </c>
-      <c r="H4" s="44">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="I4" s="44">
-        <v>14.835969061582837</v>
-      </c>
-      <c r="J4" s="45">
-        <v>17.516999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="41">
-        <v>18</v>
-      </c>
-      <c r="F5" s="42">
-        <v>355</v>
-      </c>
-      <c r="G5" s="43">
-        <v>23.161000000000001</v>
-      </c>
-      <c r="H5" s="44">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I5" s="44">
-        <v>11.35380583435758</v>
-      </c>
-      <c r="J5" s="45">
-        <v>6.915</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
-      <c r="B6" s="159"/>
-      <c r="C6" s="145" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="41">
-        <v>9</v>
-      </c>
-      <c r="F6" s="42">
-        <v>147</v>
-      </c>
-      <c r="G6" s="43">
-        <v>26.585000000000001</v>
-      </c>
-      <c r="H6" s="44">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="I6" s="44">
-        <v>18.16189516714001</v>
-      </c>
-      <c r="J6" s="45">
-        <v>23.312999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="B7" s="159"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="41">
-        <v>10</v>
-      </c>
-      <c r="F7" s="42">
-        <v>253</v>
-      </c>
-      <c r="G7" s="43">
-        <v>24.161999999999999</v>
-      </c>
-      <c r="H7" s="44">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="I7" s="44">
-        <v>12.83701437670674</v>
-      </c>
-      <c r="J7" s="45">
-        <v>9.6199999999999992</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="160"/>
-      <c r="C8" s="79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="46">
-        <v>1</v>
-      </c>
-      <c r="F8" s="47">
-        <v>26</v>
-      </c>
-      <c r="G8" s="48">
-        <v>21.808</v>
-      </c>
-      <c r="H8" s="46">
-        <v>0.41</v>
-      </c>
-      <c r="I8" s="46">
-        <v>9.7100000000000009</v>
-      </c>
-      <c r="J8" s="49">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
-      <c r="B9" s="158" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="147" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="41">
-        <v>15</v>
-      </c>
-      <c r="F9" s="42">
-        <v>222</v>
-      </c>
-      <c r="G9" s="43">
-        <v>25.977</v>
-      </c>
-      <c r="H9" s="45">
-        <v>0.251</v>
-      </c>
-      <c r="I9" s="43">
-        <v>14.41018621027294</v>
-      </c>
-      <c r="J9" s="45">
-        <v>14.013</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="41">
-        <v>8</v>
-      </c>
-      <c r="F10" s="42">
-        <v>161</v>
-      </c>
-      <c r="G10" s="43">
-        <v>28.670999999999999</v>
-      </c>
-      <c r="H10" s="45">
-        <v>0.246</v>
-      </c>
-      <c r="I10" s="43">
-        <v>10.896284161204306</v>
-      </c>
-      <c r="J10" s="45">
-        <v>9.76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="145" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="41">
-        <v>1</v>
-      </c>
-      <c r="F11" s="42">
-        <v>32</v>
-      </c>
-      <c r="G11" s="43">
-        <v>25.937999999999999</v>
-      </c>
-      <c r="H11" s="45">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="I11" s="43">
-        <v>12.070868672504577</v>
-      </c>
-      <c r="J11" s="45">
-        <v>9.8019999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
-      <c r="B12" s="159"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="41">
-        <v>3</v>
-      </c>
-      <c r="F12" s="42">
-        <v>86</v>
-      </c>
-      <c r="G12" s="43">
-        <v>26.081</v>
-      </c>
-      <c r="H12" s="45">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="I12" s="43">
-        <v>10.408689886052935</v>
-      </c>
-      <c r="J12" s="45">
-        <v>7.37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
-      <c r="B13" s="159"/>
-      <c r="C13" s="145" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="41">
-        <v>9</v>
-      </c>
-      <c r="F13" s="42">
-        <v>184</v>
-      </c>
-      <c r="G13" s="43">
-        <v>25.625</v>
-      </c>
-      <c r="H13" s="45">
-        <v>0.29499999999999998</v>
-      </c>
-      <c r="I13" s="43">
-        <v>15.628736960600049</v>
-      </c>
-      <c r="J13" s="45">
-        <v>16.039000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
-      <c r="B14" s="159"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="41">
-        <v>13</v>
-      </c>
-      <c r="F14" s="42">
-        <v>264</v>
-      </c>
-      <c r="G14" s="43">
-        <v>22.989000000000001</v>
-      </c>
-      <c r="H14" s="45">
-        <v>0.186</v>
-      </c>
-      <c r="I14" s="43">
-        <v>13.159636243359548</v>
-      </c>
-      <c r="J14" s="45">
-        <v>9.1519999999999992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
-      <c r="B15" s="159"/>
-      <c r="C15" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="41">
-        <v>3</v>
-      </c>
-      <c r="F15" s="42">
-        <v>62</v>
-      </c>
-      <c r="G15" s="43">
-        <v>22.3</v>
-      </c>
-      <c r="H15" s="50">
-        <v>0.32</v>
-      </c>
-      <c r="I15" s="42">
-        <v>11.21</v>
-      </c>
-      <c r="J15" s="50">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="81" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="41">
-        <v>3</v>
-      </c>
-      <c r="F16" s="42">
-        <v>63</v>
-      </c>
-      <c r="G16" s="42">
-        <v>24.41</v>
-      </c>
-      <c r="H16" s="50">
-        <v>0.33</v>
-      </c>
-      <c r="I16" s="42">
-        <v>10.65</v>
-      </c>
-      <c r="J16" s="50">
-        <v>6.76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
-      <c r="B17" s="160"/>
-      <c r="C17" s="83" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="46">
-        <v>2</v>
-      </c>
-      <c r="F17" s="47">
-        <v>10</v>
-      </c>
-      <c r="G17" s="48">
-        <v>23.7</v>
-      </c>
-      <c r="H17" s="49">
-        <v>1.18</v>
-      </c>
-      <c r="I17" s="47">
-        <v>15.79</v>
-      </c>
-      <c r="J17" s="49">
-        <v>14.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="155"/>
-      <c r="B18" s="158" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="156" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="51">
-        <v>1</v>
-      </c>
-      <c r="F18" s="52">
-        <v>1</v>
-      </c>
-      <c r="G18" s="53">
-        <v>26</v>
-      </c>
-      <c r="H18" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="54" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="155"/>
-      <c r="B19" s="159"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="51">
-        <v>2</v>
-      </c>
-      <c r="F19" s="52">
-        <v>44</v>
-      </c>
-      <c r="G19" s="53">
-        <v>22</v>
-      </c>
-      <c r="H19" s="55">
-        <v>0.34</v>
-      </c>
-      <c r="I19" s="55">
-        <v>10</v>
-      </c>
-      <c r="J19" s="55">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
-      <c r="B20" s="160"/>
-      <c r="C20" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="56">
-        <v>4</v>
-      </c>
-      <c r="F20" s="57">
-        <v>44</v>
-      </c>
-      <c r="G20" s="58">
-        <v>24</v>
-      </c>
-      <c r="H20" s="59">
-        <v>0.41</v>
-      </c>
-      <c r="I20" s="59">
-        <v>11</v>
-      </c>
-      <c r="J20" s="59">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
-      <c r="B21" s="161" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="162" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="88" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="60">
-        <v>14</v>
-      </c>
-      <c r="F21" s="60">
-        <v>300</v>
-      </c>
-      <c r="G21" s="61">
-        <v>28.123000000000001</v>
-      </c>
-      <c r="H21" s="62">
-        <v>0.254</v>
-      </c>
-      <c r="I21" s="62">
-        <v>15.64239374084605</v>
-      </c>
-      <c r="J21" s="63">
-        <v>19.353000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
-      <c r="B22" s="161"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="42">
-        <v>7</v>
-      </c>
-      <c r="F22" s="42">
-        <v>166</v>
-      </c>
-      <c r="G22" s="43">
-        <v>30.367000000000001</v>
-      </c>
-      <c r="H22" s="44">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="I22" s="44">
-        <v>10.262658213499735</v>
-      </c>
-      <c r="J22" s="45">
-        <v>9.7129999999999992</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
-      <c r="B23" s="161"/>
-      <c r="C23" s="147" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="42">
-        <v>1</v>
-      </c>
-      <c r="F23" s="42">
-        <v>21</v>
-      </c>
-      <c r="G23" s="43">
-        <v>27.619</v>
-      </c>
-      <c r="H23" s="44">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="I23" s="44">
-        <v>15.338917885642941</v>
-      </c>
-      <c r="J23" s="45">
-        <v>17.948</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
-      <c r="B24" s="161"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="89" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="64">
-        <v>6</v>
-      </c>
-      <c r="F24" s="64">
-        <v>119</v>
-      </c>
-      <c r="G24" s="65">
-        <v>23.42</v>
-      </c>
-      <c r="H24" s="66">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="I24" s="66">
-        <v>10.80040516644884</v>
-      </c>
-      <c r="J24" s="67">
-        <v>6.3979999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="150"/>
-      <c r="C25" s="147" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="42">
-        <v>2</v>
-      </c>
-      <c r="F25" s="42">
-        <v>2</v>
-      </c>
-      <c r="G25" s="43">
-        <v>26</v>
-      </c>
-      <c r="H25" s="45">
-        <v>2</v>
-      </c>
-      <c r="I25" s="45">
-        <v>10.878565864408424</v>
-      </c>
-      <c r="J25" s="68">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="151"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="148"/>
-      <c r="D26" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="42">
-        <v>5</v>
-      </c>
-      <c r="F26" s="42">
-        <v>103</v>
-      </c>
-      <c r="G26" s="43">
-        <v>24.427</v>
-      </c>
-      <c r="H26" s="45">
-        <v>0.246</v>
-      </c>
-      <c r="I26" s="45">
-        <v>10.232121984584271</v>
-      </c>
-      <c r="J26" s="68">
-        <v>6.2469999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="149" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="150"/>
-      <c r="C27" s="147" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="37">
-        <v>6</v>
-      </c>
-      <c r="F27" s="37">
-        <v>97</v>
-      </c>
-      <c r="G27" s="38">
-        <v>28.236999999999998</v>
-      </c>
-      <c r="H27" s="40">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="I27" s="40">
-        <v>15.628316890383017</v>
-      </c>
-      <c r="J27" s="69">
-        <v>19.474</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="151"/>
-      <c r="B28" s="152"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="89" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="64">
-        <v>4</v>
-      </c>
-      <c r="F28" s="64">
-        <v>133</v>
-      </c>
-      <c r="G28" s="65">
-        <v>25.774000000000001</v>
-      </c>
-      <c r="H28" s="67">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="I28" s="67">
-        <v>10.781039022222362</v>
-      </c>
-      <c r="J28" s="70">
-        <v>7.7210000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="153" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="154"/>
-      <c r="C29" s="83" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="71">
-        <v>2</v>
-      </c>
-      <c r="F29" s="72">
-        <v>57</v>
-      </c>
-      <c r="G29" s="73">
-        <v>27</v>
-      </c>
-      <c r="H29" s="74">
-        <v>0.4</v>
-      </c>
-      <c r="I29" s="74">
-        <v>11</v>
-      </c>
-      <c r="J29" s="75">
-        <v>8.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A2:A24"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="A27:B28"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="136" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="166"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="168" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="169"/>
-      <c r="H1" s="170"/>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="175"/>
-      <c r="B2" s="138"/>
-      <c r="C2" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="92" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="171" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="93" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="33">
-        <v>21</v>
-      </c>
-      <c r="D3" s="94">
-        <v>177.76190476190476</v>
-      </c>
-      <c r="E3" s="95">
-        <v>0.13715946228965248</v>
-      </c>
-      <c r="F3" s="96">
-        <v>20</v>
-      </c>
-      <c r="G3" s="94">
-        <v>144.25</v>
-      </c>
-      <c r="H3" s="95">
-        <v>0.16902410587679217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="171"/>
-      <c r="B4" s="93" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="33">
-        <v>19</v>
-      </c>
-      <c r="D4" s="94">
-        <v>158.15789473684211</v>
-      </c>
-      <c r="E4" s="95">
-        <v>0.15299197633573675</v>
-      </c>
-      <c r="F4" s="96">
-        <v>9</v>
-      </c>
-      <c r="G4" s="94">
-        <v>131.77777777777777</v>
-      </c>
-      <c r="H4" s="95">
-        <v>0.18361888701517706</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="171"/>
-      <c r="B5" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="33">
-        <v>1</v>
-      </c>
-      <c r="D5" s="94">
-        <v>159</v>
-      </c>
-      <c r="E5" s="95">
-        <v>0.15241074020319303</v>
-      </c>
-      <c r="F5" s="96">
-        <v>11</v>
-      </c>
-      <c r="G5" s="94">
-        <v>167.36363636363637</v>
-      </c>
-      <c r="H5" s="95">
-        <v>0.1447943425395897</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="172" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="32">
-        <v>18</v>
-      </c>
-      <c r="D6" s="97">
-        <v>180.22222222222223</v>
-      </c>
-      <c r="E6" s="98">
-        <v>0.16261243834771885</v>
-      </c>
-      <c r="F6" s="99">
-        <v>18</v>
-      </c>
-      <c r="G6" s="97">
-        <v>140.77777777777777</v>
-      </c>
-      <c r="H6" s="98">
-        <v>0.20817472375690607</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="173"/>
-      <c r="B7" s="93" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="34">
-        <v>17</v>
-      </c>
-      <c r="D7" s="100">
-        <v>231</v>
-      </c>
-      <c r="E7" s="101">
-        <v>0.13518614718614719</v>
-      </c>
-      <c r="F7" s="102">
-        <v>17</v>
-      </c>
-      <c r="G7" s="100">
-        <v>164.41176470588235</v>
-      </c>
-      <c r="H7" s="101">
-        <v>0.1899377459749553</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
few more updates before submitting. FIXED TYPO IN FIG3
</commit_message>
<xml_diff>
--- a/doc/MainTables.xlsx
+++ b/doc/MainTables.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
   <si>
     <t>Species</t>
   </si>
@@ -605,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -824,226 +824,266 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1051,7 +1091,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1137,79 +1177,304 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1230,33 +1495,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1275,206 +1513,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1764,7 +1840,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,201 +1852,201 @@
     <col min="15" max="15" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="132" t="s">
+      <c r="E1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="132" t="s">
+      <c r="F1" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="131" t="s">
+      <c r="H1" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="131" t="s">
+      <c r="I1" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="131" t="s">
+      <c r="J1" s="110" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="138">
+      <c r="E2" s="78">
         <v>14</v>
       </c>
-      <c r="F2" s="138">
+      <c r="F2" s="78">
         <v>184</v>
       </c>
-      <c r="G2" s="139">
+      <c r="G2" s="79">
         <v>24.701000000000001</v>
       </c>
-      <c r="H2" s="139">
+      <c r="H2" s="79">
         <v>0.26700000000000002</v>
       </c>
-      <c r="I2" s="139">
+      <c r="I2" s="79">
         <v>14.638271224837814</v>
       </c>
-      <c r="J2" s="140">
+      <c r="J2" s="84">
         <v>13.074</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
-      <c r="B3" s="130"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="106" t="s">
+      <c r="A3" s="130"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="107">
+      <c r="E3" s="72">
         <v>11</v>
       </c>
-      <c r="F3" s="107">
+      <c r="F3" s="72">
         <v>222</v>
       </c>
-      <c r="G3" s="108">
+      <c r="G3" s="73">
         <v>23.382999999999999</v>
       </c>
-      <c r="H3" s="108">
+      <c r="H3" s="73">
         <v>0.18</v>
       </c>
-      <c r="I3" s="108">
+      <c r="I3" s="73">
         <v>11.479933887268658</v>
       </c>
-      <c r="J3" s="142">
+      <c r="J3" s="83">
         <v>7.2060000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
-      <c r="B4" s="130"/>
-      <c r="C4" s="141" t="s">
+      <c r="A4" s="130"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="107">
+      <c r="E4" s="72">
         <v>12</v>
       </c>
-      <c r="F4" s="107">
+      <c r="F4" s="72">
         <v>318</v>
       </c>
-      <c r="G4" s="108">
+      <c r="G4" s="73">
         <v>28.210999999999999</v>
       </c>
-      <c r="H4" s="108">
+      <c r="H4" s="73">
         <v>0.23499999999999999</v>
       </c>
-      <c r="I4" s="108">
+      <c r="I4" s="73">
         <v>14.835969061582837</v>
       </c>
-      <c r="J4" s="142">
+      <c r="J4" s="83">
         <v>17.516999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="122"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="106" t="s">
+      <c r="A5" s="130"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="107">
+      <c r="E5" s="72">
         <v>18</v>
       </c>
-      <c r="F5" s="107">
+      <c r="F5" s="72">
         <v>355</v>
       </c>
-      <c r="G5" s="108">
+      <c r="G5" s="73">
         <v>23.161000000000001</v>
       </c>
-      <c r="H5" s="108">
+      <c r="H5" s="73">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I5" s="108">
+      <c r="I5" s="73">
         <v>11.35380583435758</v>
       </c>
-      <c r="J5" s="142">
+      <c r="J5" s="83">
         <v>6.915</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
-      <c r="B6" s="130"/>
-      <c r="C6" s="141" t="s">
+      <c r="A6" s="130"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="107">
+      <c r="E6" s="72">
         <v>9</v>
       </c>
-      <c r="F6" s="107">
+      <c r="F6" s="72">
         <v>147</v>
       </c>
-      <c r="G6" s="108">
+      <c r="G6" s="73">
         <v>26.585000000000001</v>
       </c>
-      <c r="H6" s="108">
+      <c r="H6" s="73">
         <v>0.39800000000000002</v>
       </c>
-      <c r="I6" s="108">
+      <c r="I6" s="73">
         <v>18.16189516714001</v>
       </c>
-      <c r="J6" s="142">
+      <c r="J6" s="83">
         <v>23.312999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="106" t="s">
+      <c r="A7" s="130"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="107">
+      <c r="E7" s="72">
         <v>10</v>
       </c>
-      <c r="F7" s="107">
+      <c r="F7" s="72">
         <v>253</v>
       </c>
-      <c r="G7" s="108">
+      <c r="G7" s="73">
         <v>24.161999999999999</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="73">
         <v>0.19500000000000001</v>
       </c>
-      <c r="I7" s="108">
+      <c r="I7" s="73">
         <v>12.83701437670674</v>
       </c>
-      <c r="J7" s="142">
+      <c r="J7" s="83">
         <v>9.6199999999999992</v>
       </c>
       <c r="L7" s="2"/>
@@ -1984,31 +2060,31 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="122"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="143" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="130"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="144" t="s">
+      <c r="D8" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="145">
+      <c r="E8" s="80">
         <v>1</v>
       </c>
-      <c r="F8" s="145">
+      <c r="F8" s="80">
         <v>26</v>
       </c>
-      <c r="G8" s="146">
+      <c r="G8" s="81">
         <v>21.808</v>
       </c>
-      <c r="H8" s="145">
+      <c r="H8" s="80">
         <v>0.41</v>
       </c>
-      <c r="I8" s="145">
+      <c r="I8" s="80">
         <v>9.7100000000000009</v>
       </c>
-      <c r="J8" s="147">
+      <c r="J8" s="91">
         <v>4.4800000000000004</v>
       </c>
       <c r="L8" s="5"/>
@@ -2023,444 +2099,440 @@
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="121" t="s">
+      <c r="A9" s="130"/>
+      <c r="B9" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="135">
+      <c r="E9" s="96">
         <v>15</v>
       </c>
-      <c r="F9" s="135">
+      <c r="F9" s="96">
         <v>222</v>
       </c>
-      <c r="G9" s="136">
+      <c r="G9" s="97">
         <v>25.977</v>
       </c>
-      <c r="H9" s="136">
+      <c r="H9" s="97">
         <v>0.251</v>
       </c>
-      <c r="I9" s="136">
+      <c r="I9" s="97">
         <v>14.41018621027294</v>
       </c>
-      <c r="J9" s="136">
+      <c r="J9" s="98">
         <v>14.013</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="106" t="s">
+      <c r="A10" s="130"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="107">
+      <c r="E10" s="72">
         <v>8</v>
       </c>
-      <c r="F10" s="107">
+      <c r="F10" s="72">
         <v>161</v>
       </c>
-      <c r="G10" s="108">
+      <c r="G10" s="73">
         <v>28.670999999999999</v>
       </c>
-      <c r="H10" s="108">
+      <c r="H10" s="73">
         <v>0.246</v>
       </c>
-      <c r="I10" s="108">
+      <c r="I10" s="73">
         <v>10.896284161204306</v>
       </c>
-      <c r="J10" s="108">
+      <c r="J10" s="83">
         <v>9.76</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="122"/>
-      <c r="C11" s="118" t="s">
+      <c r="A11" s="130"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="106" t="s">
+      <c r="D11" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="107">
+      <c r="E11" s="72">
         <v>1</v>
       </c>
-      <c r="F11" s="107">
+      <c r="F11" s="72">
         <v>32</v>
       </c>
-      <c r="G11" s="108">
+      <c r="G11" s="73">
         <v>25.937999999999999</v>
       </c>
-      <c r="H11" s="108">
+      <c r="H11" s="73">
         <v>0.55300000000000005</v>
       </c>
-      <c r="I11" s="108">
+      <c r="I11" s="73">
         <v>12.070868672504577</v>
       </c>
-      <c r="J11" s="108">
+      <c r="J11" s="83">
         <v>9.8019999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="106" t="s">
+      <c r="A12" s="130"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="107">
+      <c r="E12" s="72">
         <v>3</v>
       </c>
-      <c r="F12" s="107">
+      <c r="F12" s="72">
         <v>86</v>
       </c>
-      <c r="G12" s="108">
+      <c r="G12" s="73">
         <v>26.081</v>
       </c>
-      <c r="H12" s="108">
+      <c r="H12" s="73">
         <v>0.29299999999999998</v>
       </c>
-      <c r="I12" s="108">
+      <c r="I12" s="73">
         <v>10.408689886052935</v>
       </c>
-      <c r="J12" s="108">
+      <c r="J12" s="83">
         <v>7.37</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="118" t="s">
+      <c r="A13" s="130"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="107">
+      <c r="E13" s="72">
         <v>9</v>
       </c>
-      <c r="F13" s="107">
+      <c r="F13" s="72">
         <v>184</v>
       </c>
-      <c r="G13" s="108">
+      <c r="G13" s="73">
         <v>25.625</v>
       </c>
-      <c r="H13" s="108">
+      <c r="H13" s="73">
         <v>0.29499999999999998</v>
       </c>
-      <c r="I13" s="108">
+      <c r="I13" s="73">
         <v>15.628736960600049</v>
       </c>
-      <c r="J13" s="108">
+      <c r="J13" s="83">
         <v>16.039000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="122"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="106" t="s">
+      <c r="A14" s="130"/>
+      <c r="B14" s="132"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="107">
+      <c r="E14" s="72">
         <v>13</v>
       </c>
-      <c r="F14" s="107">
+      <c r="F14" s="72">
         <v>264</v>
       </c>
-      <c r="G14" s="108">
+      <c r="G14" s="73">
         <v>22.989000000000001</v>
       </c>
-      <c r="H14" s="108">
+      <c r="H14" s="73">
         <v>0.186</v>
       </c>
-      <c r="I14" s="108">
+      <c r="I14" s="73">
         <v>13.159636243359548</v>
       </c>
-      <c r="J14" s="108">
+      <c r="J14" s="83">
         <v>9.1519999999999992</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="122"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="109" t="s">
+      <c r="A15" s="130"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="106" t="s">
+      <c r="D15" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="107">
+      <c r="E15" s="72">
         <v>3</v>
       </c>
-      <c r="F15" s="107">
+      <c r="F15" s="72">
         <v>62</v>
       </c>
-      <c r="G15" s="108">
+      <c r="G15" s="73">
         <v>22.3</v>
       </c>
-      <c r="H15" s="107">
+      <c r="H15" s="72">
         <v>0.32</v>
       </c>
-      <c r="I15" s="107">
+      <c r="I15" s="72">
         <v>11.21</v>
       </c>
-      <c r="J15" s="107">
+      <c r="J15" s="85">
         <v>6.25</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="122"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="109" t="s">
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="106" t="s">
+      <c r="D16" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="107">
+      <c r="E16" s="72">
         <v>3</v>
       </c>
-      <c r="F16" s="107">
+      <c r="F16" s="72">
         <v>63</v>
       </c>
-      <c r="G16" s="107">
+      <c r="G16" s="72">
         <v>24.41</v>
       </c>
-      <c r="H16" s="107">
+      <c r="H16" s="72">
         <v>0.33</v>
       </c>
-      <c r="I16" s="107">
+      <c r="I16" s="72">
         <v>10.65</v>
       </c>
-      <c r="J16" s="107">
+      <c r="J16" s="85">
         <v>6.76</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="112" t="s">
+      <c r="A17" s="130"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D17" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="110">
+      <c r="E17" s="99">
         <v>2</v>
       </c>
-      <c r="F17" s="110">
+      <c r="F17" s="99">
         <v>10</v>
       </c>
-      <c r="G17" s="111">
+      <c r="G17" s="100">
         <v>23.7</v>
       </c>
-      <c r="H17" s="110">
+      <c r="H17" s="99">
         <v>1.18</v>
       </c>
-      <c r="I17" s="110">
+      <c r="I17" s="99">
         <v>15.79</v>
       </c>
-      <c r="J17" s="110">
+      <c r="J17" s="101">
         <v>14.01</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="122"/>
-      <c r="B18" s="121" t="s">
+      <c r="A18" s="130"/>
+      <c r="B18" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="114" t="s">
+      <c r="D18" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="115">
+      <c r="E18" s="92">
         <v>1</v>
       </c>
-      <c r="F18" s="115">
+      <c r="F18" s="92">
         <v>1</v>
       </c>
-      <c r="G18" s="116">
+      <c r="G18" s="93">
         <v>26</v>
       </c>
-      <c r="H18" s="117" t="s">
+      <c r="H18" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="117" t="s">
-        <v>42</v>
-      </c>
+      <c r="I18" s="94"/>
+      <c r="J18" s="95"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="122"/>
-      <c r="B19" s="122"/>
+      <c r="A19" s="130"/>
+      <c r="B19" s="132"/>
       <c r="C19" s="119"/>
-      <c r="D19" s="114" t="s">
+      <c r="D19" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="115">
+      <c r="E19" s="76">
         <v>2</v>
       </c>
-      <c r="F19" s="115">
+      <c r="F19" s="76">
         <v>44</v>
       </c>
-      <c r="G19" s="116">
+      <c r="G19" s="77">
         <v>22</v>
       </c>
-      <c r="H19" s="116">
+      <c r="H19" s="77">
         <v>0.34</v>
       </c>
-      <c r="I19" s="116">
+      <c r="I19" s="77">
         <v>10</v>
       </c>
-      <c r="J19" s="116">
+      <c r="J19" s="86">
         <v>5.2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="122"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="112" t="s">
+      <c r="A20" s="130"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="114" t="s">
+      <c r="D20" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="115">
+      <c r="E20" s="76">
         <v>4</v>
       </c>
-      <c r="F20" s="115">
+      <c r="F20" s="76">
         <v>44</v>
       </c>
-      <c r="G20" s="116">
+      <c r="G20" s="77">
         <v>24</v>
       </c>
-      <c r="H20" s="116">
+      <c r="H20" s="77">
         <v>0.41</v>
       </c>
-      <c r="I20" s="116">
+      <c r="I20" s="77">
         <v>11</v>
       </c>
-      <c r="J20" s="116">
+      <c r="J20" s="86">
         <v>7.5</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="122"/>
-      <c r="B21" s="121" t="s">
+      <c r="A21" s="130"/>
+      <c r="B21" s="131" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="113" t="s">
+      <c r="D21" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="110">
+      <c r="E21" s="74">
         <v>14</v>
       </c>
-      <c r="F21" s="110">
+      <c r="F21" s="74">
         <v>300</v>
       </c>
-      <c r="G21" s="111">
+      <c r="G21" s="75">
         <v>28.123000000000001</v>
       </c>
-      <c r="H21" s="111">
+      <c r="H21" s="75">
         <v>0.254</v>
       </c>
-      <c r="I21" s="111">
+      <c r="I21" s="75">
         <v>15.64239374084605</v>
       </c>
-      <c r="J21" s="111">
+      <c r="J21" s="87">
         <v>19.353000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="106" t="s">
+      <c r="A22" s="130"/>
+      <c r="B22" s="132"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="107">
+      <c r="E22" s="72">
         <v>7</v>
       </c>
-      <c r="F22" s="107">
+      <c r="F22" s="72">
         <v>166</v>
       </c>
-      <c r="G22" s="108">
+      <c r="G22" s="73">
         <v>30.367000000000001</v>
       </c>
-      <c r="H22" s="108">
+      <c r="H22" s="73">
         <v>0.24199999999999999</v>
       </c>
-      <c r="I22" s="108">
+      <c r="I22" s="73">
         <v>10.262658213499735</v>
       </c>
-      <c r="J22" s="108">
+      <c r="J22" s="83">
         <v>9.7129999999999992</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="118" t="s">
+      <c r="A23" s="130"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="106" t="s">
+      <c r="D23" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="107">
+      <c r="E23" s="72">
         <v>1</v>
       </c>
-      <c r="F23" s="107">
+      <c r="F23" s="72">
         <v>21</v>
       </c>
-      <c r="G23" s="108">
+      <c r="G23" s="73">
         <v>27.619</v>
       </c>
-      <c r="H23" s="108">
+      <c r="H23" s="73">
         <v>0.92400000000000004</v>
       </c>
-      <c r="I23" s="108">
+      <c r="I23" s="73">
         <v>15.338917885642941</v>
       </c>
-      <c r="J23" s="108">
+      <c r="J23" s="83">
         <v>17.948</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="106" t="s">
+      <c r="A24" s="130"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="107">
+      <c r="E24" s="72">
         <v>6</v>
       </c>
-      <c r="F24" s="107">
+      <c r="F24" s="72">
         <v>119</v>
       </c>
-      <c r="G24" s="108">
+      <c r="G24" s="73">
         <v>23.42</v>
       </c>
-      <c r="H24" s="108">
+      <c r="H24" s="73">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I24" s="108">
+      <c r="I24" s="73">
         <v>10.80040516644884</v>
       </c>
-      <c r="J24" s="108">
+      <c r="J24" s="83">
         <v>6.3979999999999997</v>
       </c>
     </row>
@@ -2469,54 +2541,54 @@
         <v>92</v>
       </c>
       <c r="B25" s="125"/>
-      <c r="C25" s="118" t="s">
+      <c r="C25" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="106" t="s">
+      <c r="D25" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="107">
+      <c r="E25" s="72">
         <v>2</v>
       </c>
-      <c r="F25" s="107">
+      <c r="F25" s="72">
         <v>2</v>
       </c>
-      <c r="G25" s="108">
+      <c r="G25" s="73">
         <v>26</v>
       </c>
-      <c r="H25" s="108">
+      <c r="H25" s="73">
         <v>2</v>
       </c>
-      <c r="I25" s="108">
+      <c r="I25" s="73">
         <v>10.878565864408424</v>
       </c>
-      <c r="J25" s="108">
+      <c r="J25" s="83">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="126"/>
       <c r="B26" s="127"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="106" t="s">
+      <c r="C26" s="117"/>
+      <c r="D26" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="107">
+      <c r="E26" s="72">
         <v>5</v>
       </c>
-      <c r="F26" s="107">
+      <c r="F26" s="72">
         <v>103</v>
       </c>
-      <c r="G26" s="108">
+      <c r="G26" s="73">
         <v>24.427</v>
       </c>
-      <c r="H26" s="108">
+      <c r="H26" s="73">
         <v>0.246</v>
       </c>
-      <c r="I26" s="108">
+      <c r="I26" s="73">
         <v>10.232121984584271</v>
       </c>
-      <c r="J26" s="108">
+      <c r="J26" s="83">
         <v>6.2469999999999999</v>
       </c>
     </row>
@@ -2525,54 +2597,54 @@
         <v>21</v>
       </c>
       <c r="B27" s="125"/>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="106" t="s">
+      <c r="D27" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="107">
+      <c r="E27" s="72">
         <v>6</v>
       </c>
-      <c r="F27" s="107">
+      <c r="F27" s="72">
         <v>97</v>
       </c>
-      <c r="G27" s="108">
+      <c r="G27" s="73">
         <v>28.236999999999998</v>
       </c>
-      <c r="H27" s="108">
+      <c r="H27" s="73">
         <v>0.44800000000000001</v>
       </c>
-      <c r="I27" s="108">
+      <c r="I27" s="73">
         <v>15.628316890383017</v>
       </c>
-      <c r="J27" s="108">
+      <c r="J27" s="83">
         <v>19.474</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="126"/>
       <c r="B28" s="127"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="106" t="s">
+      <c r="C28" s="117"/>
+      <c r="D28" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="107">
+      <c r="E28" s="72">
         <v>4</v>
       </c>
-      <c r="F28" s="107">
+      <c r="F28" s="72">
         <v>133</v>
       </c>
-      <c r="G28" s="108">
+      <c r="G28" s="73">
         <v>25.774000000000001</v>
       </c>
-      <c r="H28" s="108">
+      <c r="H28" s="73">
         <v>0.24099999999999999</v>
       </c>
-      <c r="I28" s="108">
+      <c r="I28" s="73">
         <v>10.781039022222362</v>
       </c>
-      <c r="J28" s="108">
+      <c r="J28" s="83">
         <v>7.7210000000000001</v>
       </c>
     </row>
@@ -2581,33 +2653,33 @@
         <v>43</v>
       </c>
       <c r="B29" s="129"/>
-      <c r="C29" s="112" t="s">
+      <c r="C29" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="113" t="s">
+      <c r="D29" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="115">
+      <c r="E29" s="88">
         <v>2</v>
       </c>
-      <c r="F29" s="115">
+      <c r="F29" s="88">
         <v>57</v>
       </c>
-      <c r="G29" s="116">
+      <c r="G29" s="89">
         <v>27</v>
       </c>
-      <c r="H29" s="116">
+      <c r="H29" s="89">
         <v>0.4</v>
       </c>
-      <c r="I29" s="116">
+      <c r="I29" s="89">
         <v>11</v>
       </c>
-      <c r="J29" s="116">
+      <c r="J29" s="90">
         <v>8.9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="19">
     <mergeCell ref="A25:B26"/>
     <mergeCell ref="A27:B28"/>
     <mergeCell ref="A29:B29"/>
@@ -2616,6 +2688,17 @@
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B9:B17"/>
     <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2626,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A9" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,10 +2740,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="134" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="137" t="s">
         <v>103</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -2674,8 +2757,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="135"/>
+      <c r="B3" s="138"/>
       <c r="C3" s="19"/>
       <c r="D3" s="4" t="s">
         <v>44</v>
@@ -2683,8 +2766,8 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="64"/>
+      <c r="A4" s="136"/>
+      <c r="B4" s="139"/>
       <c r="C4" s="17"/>
       <c r="D4" s="4" t="s">
         <v>46</v>
@@ -2692,10 +2775,10 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="134" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="140" t="s">
         <v>103</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -2707,8 +2790,8 @@
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="19"/>
       <c r="D6" s="10" t="s">
         <v>44</v>
@@ -2716,8 +2799,8 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="19"/>
       <c r="D7" s="10" t="s">
         <v>31</v>
@@ -2725,8 +2808,8 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="66"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="19"/>
       <c r="D8" s="10" t="s">
         <v>46</v>
@@ -2734,8 +2817,8 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
-      <c r="B9" s="66"/>
+      <c r="A9" s="135"/>
+      <c r="B9" s="141"/>
       <c r="C9" s="19"/>
       <c r="D9" s="10" t="s">
         <v>47</v>
@@ -2743,8 +2826,8 @@
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="17"/>
       <c r="D10" s="11" t="s">
         <v>48</v>
@@ -2752,10 +2835,10 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="140" t="s">
         <v>103</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -2767,8 +2850,8 @@
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="19"/>
       <c r="D12" s="10" t="s">
         <v>31</v>
@@ -2776,8 +2859,8 @@
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="67"/>
+      <c r="A13" s="136"/>
+      <c r="B13" s="142"/>
       <c r="C13" s="17"/>
       <c r="D13" s="11" t="s">
         <v>48</v>
@@ -2785,7 +2868,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="134" t="s">
         <v>101</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -2800,7 +2883,7 @@
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="24"/>
       <c r="C15" s="28"/>
       <c r="D15" s="31" t="s">
@@ -2809,7 +2892,7 @@
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
+      <c r="A16" s="136"/>
       <c r="B16" s="25"/>
       <c r="C16" s="22"/>
       <c r="D16" s="32" t="s">
@@ -2818,7 +2901,7 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="134" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="20" t="s">
@@ -2833,7 +2916,7 @@
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="24"/>
       <c r="C18" s="28"/>
       <c r="D18" s="31" t="s">
@@ -2842,7 +2925,7 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
+      <c r="A19" s="136"/>
       <c r="B19" s="25"/>
       <c r="C19" s="22"/>
       <c r="D19" s="32" t="s">
@@ -2851,7 +2934,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="134" t="s">
         <v>102</v>
       </c>
       <c r="B20" s="26" t="s">
@@ -2866,14 +2949,14 @@
       <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
+      <c r="A21" s="136"/>
       <c r="B21" s="27"/>
       <c r="C21" s="22"/>
       <c r="D21" s="33"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="134" t="s">
         <v>102</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -2888,7 +2971,7 @@
       <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="76"/>
+      <c r="A23" s="136"/>
       <c r="B23" s="27"/>
       <c r="C23" s="22"/>
       <c r="D23" s="33"/>
@@ -2917,7 +3000,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="H7" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2932,166 +3015,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="154" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80" t="s">
+      <c r="D1" s="144"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="146" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="82"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="148"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="103"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="96" t="s">
+      <c r="A2" s="155"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="97" t="s">
+      <c r="G2" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="H2" s="57" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="149" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="64">
         <v>21</v>
       </c>
-      <c r="D3" s="84">
+      <c r="D3" s="58">
         <v>177.76190476190476</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="59">
         <v>0.13715946228965248</v>
       </c>
-      <c r="F3" s="93">
+      <c r="F3" s="67">
         <v>20</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="58">
         <v>144.25</v>
       </c>
-      <c r="H3" s="85">
+      <c r="H3" s="59">
         <v>0.16902410587679217</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
+      <c r="A4" s="149"/>
       <c r="B4" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="64">
         <v>19</v>
       </c>
-      <c r="D4" s="84">
+      <c r="D4" s="58">
         <v>158.15789473684211</v>
       </c>
-      <c r="E4" s="85">
+      <c r="E4" s="59">
         <v>0.15299197633573675</v>
       </c>
-      <c r="F4" s="93">
+      <c r="F4" s="67">
         <v>9</v>
       </c>
-      <c r="G4" s="84">
+      <c r="G4" s="58">
         <v>131.77777777777777</v>
       </c>
-      <c r="H4" s="85">
+      <c r="H4" s="59">
         <v>0.18361888701517706</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
+      <c r="A5" s="149"/>
       <c r="B5" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="90">
+      <c r="C5" s="64">
         <v>1</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="58">
         <v>159</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="59">
         <v>0.15241074020319303</v>
       </c>
-      <c r="F5" s="93">
+      <c r="F5" s="67">
         <v>11</v>
       </c>
-      <c r="G5" s="84">
+      <c r="G5" s="58">
         <v>167.36363636363637</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="59">
         <v>0.1447943425395897</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="150" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="91">
+      <c r="C6" s="65">
         <v>18</v>
       </c>
-      <c r="D6" s="86">
+      <c r="D6" s="60">
         <v>180.22222222222223</v>
       </c>
-      <c r="E6" s="87">
+      <c r="E6" s="61">
         <v>0.16261243834771885</v>
       </c>
-      <c r="F6" s="94">
+      <c r="F6" s="68">
         <v>18</v>
       </c>
-      <c r="G6" s="86">
+      <c r="G6" s="60">
         <v>140.77777777777777</v>
       </c>
-      <c r="H6" s="87">
+      <c r="H6" s="61">
         <v>0.20817472375690607</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
+      <c r="A7" s="151"/>
       <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="92">
+      <c r="C7" s="66">
         <v>17</v>
       </c>
-      <c r="D7" s="88">
+      <c r="D7" s="62">
         <v>231</v>
       </c>
-      <c r="E7" s="89">
+      <c r="E7" s="63">
         <v>0.13518614718614719</v>
       </c>
-      <c r="F7" s="95">
+      <c r="F7" s="69">
         <v>17</v>
       </c>
-      <c r="G7" s="88">
+      <c r="G7" s="62">
         <v>164.41176470588235</v>
       </c>
-      <c r="H7" s="89">
+      <c r="H7" s="63">
         <v>0.1899377459749553</v>
       </c>
     </row>
@@ -3114,7 +3197,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,286 +3210,286 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="112" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="114" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="157"/>
+      <c r="B3" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="157"/>
+      <c r="B4" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="45" t="s">
+      <c r="A5" s="158"/>
+      <c r="B5" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="159" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="39" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="49" t="s">
+      <c r="A7" s="160"/>
+      <c r="B7" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="160"/>
+      <c r="B8" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="42" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="160"/>
+      <c r="B9" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="49" t="s">
+      <c r="A10" s="160"/>
+      <c r="B10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="52" t="s">
+      <c r="A11" s="161"/>
+      <c r="B11" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="158"/>
+      <c r="B13" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="156" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="39" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
-      <c r="B15" s="55" t="s">
+      <c r="A15" s="158"/>
+      <c r="B15" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="39" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="54" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>